<commit_message>
ADD SCH AND RATING COMPARE
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1617"/>
+  <dimension ref="A1:H1628"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H238" t="inlineStr"/>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H256" t="inlineStr"/>
@@ -10198,7 +10198,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H257" t="inlineStr"/>
@@ -12288,7 +12288,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H312" t="inlineStr"/>
@@ -12364,7 +12364,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H314" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>29,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H339" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H464" t="inlineStr"/>
@@ -20078,7 +20078,7 @@
       </c>
       <c r="G517" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>25,00</t>
         </is>
       </c>
       <c r="H517" t="inlineStr"/>
@@ -36114,7 +36114,7 @@
       </c>
       <c r="G939" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>200,00</t>
         </is>
       </c>
       <c r="H939" t="inlineStr"/>
@@ -37862,7 +37862,7 @@
       </c>
       <c r="G985" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>41,777</t>
         </is>
       </c>
       <c r="H985" t="inlineStr"/>
@@ -37900,7 +37900,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>61,293</t>
+          <t>50,886</t>
         </is>
       </c>
       <c r="H986" t="inlineStr"/>
@@ -37938,7 +37938,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>28,014</t>
         </is>
       </c>
       <c r="H987" t="inlineStr"/>
@@ -37976,7 +37976,7 @@
       </c>
       <c r="G988" t="inlineStr">
         <is>
-          <t>45,28</t>
+          <t>146,56099999999998</t>
         </is>
       </c>
       <c r="H988" t="inlineStr"/>
@@ -38014,7 +38014,7 @@
       </c>
       <c r="G989" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>821,582</t>
         </is>
       </c>
       <c r="H989" t="inlineStr"/>
@@ -38052,7 +38052,7 @@
       </c>
       <c r="G990" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>116,204</t>
         </is>
       </c>
       <c r="H990" t="inlineStr"/>
@@ -39078,7 +39078,7 @@
       </c>
       <c r="G1017" t="inlineStr">
         <is>
-          <t>55,00</t>
+          <t>292,8</t>
         </is>
       </c>
       <c r="H1017" t="inlineStr"/>
@@ -39116,7 +39116,7 @@
       </c>
       <c r="G1018" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>454,00</t>
         </is>
       </c>
       <c r="H1018" t="inlineStr"/>
@@ -39154,7 +39154,7 @@
       </c>
       <c r="G1019" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>506,00</t>
         </is>
       </c>
       <c r="H1019" t="inlineStr"/>
@@ -39458,7 +39458,7 @@
       </c>
       <c r="G1027" t="inlineStr">
         <is>
-          <t>2,17</t>
+          <t>2,76</t>
         </is>
       </c>
       <c r="H1027" t="inlineStr"/>
@@ -39534,7 +39534,7 @@
       </c>
       <c r="G1029" t="inlineStr">
         <is>
-          <t>135,57</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1029" t="inlineStr"/>
@@ -39572,7 +39572,7 @@
       </c>
       <c r="G1030" t="inlineStr">
         <is>
-          <t>1492,55</t>
+          <t>198,96</t>
         </is>
       </c>
       <c r="H1030" t="inlineStr"/>
@@ -39610,7 +39610,7 @@
       </c>
       <c r="G1031" t="inlineStr">
         <is>
-          <t>254,46</t>
+          <t>4202,570000000001</t>
         </is>
       </c>
       <c r="H1031" t="inlineStr"/>
@@ -39648,7 +39648,7 @@
       </c>
       <c r="G1032" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>582,4300000000001</t>
         </is>
       </c>
       <c r="H1032" t="inlineStr"/>
@@ -39724,7 +39724,7 @@
       </c>
       <c r="G1034" t="inlineStr">
         <is>
-          <t>729,84</t>
+          <t>0,5</t>
         </is>
       </c>
       <c r="H1034" t="inlineStr"/>
@@ -40522,7 +40522,7 @@
       </c>
       <c r="G1055" t="inlineStr">
         <is>
-          <t>2,17</t>
+          <t>2,76</t>
         </is>
       </c>
       <c r="H1055" t="inlineStr"/>
@@ -40598,7 +40598,7 @@
       </c>
       <c r="G1057" t="inlineStr">
         <is>
-          <t>135,57</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1057" t="inlineStr"/>
@@ -40636,7 +40636,7 @@
       </c>
       <c r="G1058" t="inlineStr">
         <is>
-          <t>1492,55</t>
+          <t>198,96</t>
         </is>
       </c>
       <c r="H1058" t="inlineStr"/>
@@ -40674,7 +40674,7 @@
       </c>
       <c r="G1059" t="inlineStr">
         <is>
-          <t>254,46</t>
+          <t>4202,570000000001</t>
         </is>
       </c>
       <c r="H1059" t="inlineStr"/>
@@ -40712,7 +40712,7 @@
       </c>
       <c r="G1060" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>582,4300000000001</t>
         </is>
       </c>
       <c r="H1060" t="inlineStr"/>
@@ -40788,7 +40788,7 @@
       </c>
       <c r="G1062" t="inlineStr">
         <is>
-          <t>729,84</t>
+          <t>0,5</t>
         </is>
       </c>
       <c r="H1062" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>1,628</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>5,64</t>
+          <t>5,84</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>0,604</t>
+          <t>81,64</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43068,7 +43068,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10,2</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -43144,7 +43144,7 @@
       </c>
       <c r="G1124" t="inlineStr">
         <is>
-          <t>2,715</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1124" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>62,57</t>
+          <t>156,37</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>62,57</t>
+          <t>156,37</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>62,57</t>
+          <t>156,37</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>62,57</t>
+          <t>156,37</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>555,6</t>
+          <t>172,8</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>27,00</t>
+          <t>15,6</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>468,3</t>
+          <t>962,325</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>78,76</t>
+          <t>153,01</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 12", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-30</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61316,7 +61316,7 @@
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>18,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -61348,17 +61348,17 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2-1/2 ", S-30</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -61390,7 +61390,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 12 ", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 4 ", S-30</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -61400,7 +61400,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>12,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,7 +61432,7 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3 ", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 6 ", S-40</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
@@ -61442,7 +61442,7 @@
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>127,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,7 +61474,7 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4 ", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 8 ", S-20</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
@@ -61484,7 +61484,7 @@
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>77,00</t>
+          <t>13,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,17 +61516,17 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6 ", S-40</t>
+          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE 6"</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 12 "</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X120MMLG</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61568,7 +61568,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -61600,7 +61600,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 3 "</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -61610,7 +61610,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,7 +61642,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8 " THK, 12 "</t>
+          <t>SUMINISTRO DE TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -61652,7 +61652,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,7 +61684,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12 " X 1 "</t>
+          <t>SUMINISTRO DE CONC. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X4"</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -61694,7 +61694,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,7 +61726,7 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12 " X 1/2 "</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X6"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
@@ -61736,7 +61736,7 @@
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,7 +61768,7 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12 " X 3/4 "</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 4"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
@@ -61778,7 +61778,7 @@
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,7 +61810,7 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4 " X 3/4 "</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 6"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
@@ -61820,7 +61820,7 @@
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -61852,7 +61852,7 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 6 " X 3/4 "</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 8"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
@@ -61862,7 +61862,7 @@
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -61894,7 +61894,7 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 12"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A53 GR. B, 3/4 ", S-160</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
@@ -61904,7 +61904,7 @@
       </c>
       <c r="G1616" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1616" t="inlineStr">
@@ -61936,7 +61936,7 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 12" X 3 ", S-30 X S-40</t>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1/2 ", S-XXS</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
@@ -61950,6 +61950,468 @@
         </is>
       </c>
       <c r="H1617" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1618" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1½ ", S-160</t>
+        </is>
+      </c>
+      <c r="F1618" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1618" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1618" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1619">
+      <c r="A1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1619" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 3/4 ", S-160</t>
+        </is>
+      </c>
+      <c r="F1619" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1619" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1619" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1620" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 4"</t>
+        </is>
+      </c>
+      <c r="F1620" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1620" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1620" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1621" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE REDUCER TEE, SCH20 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 4"</t>
+        </is>
+      </c>
+      <c r="F1621" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1621" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1621" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1622">
+      <c r="A1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1622" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 80 X SCH 80, PEXPE, ASTM A-234 GR WCB, MSS SP-95 1-1/2"X1"</t>
+        </is>
+      </c>
+      <c r="F1622" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1622" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1622" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1623">
+      <c r="A1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1623" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 6 " X 1/2 "</t>
+        </is>
+      </c>
+      <c r="F1623" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1623" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1623" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1624">
+      <c r="A1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1624" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 4 ", S-30</t>
+        </is>
+      </c>
+      <c r="F1624" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1624" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1624" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1625" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 8 ", S-20</t>
+        </is>
+      </c>
+      <c r="F1625" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1625" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1625" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1626" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 6" X 2-1/2 ", S-40 X S-30</t>
+        </is>
+      </c>
+      <c r="F1626" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1626" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1626" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PREFABRICACIÓN EN TALLER DE TUBERÍA DE ACERO AL CARBÓN DE Ø 2-1/2" </t>
+        </is>
+      </c>
+      <c r="F1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1627" t="inlineStr">
+        <is>
+          <t>15,28</t>
+        </is>
+      </c>
+      <c r="H1627" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1628" t="inlineStr">
+        <is>
+          <t>MONTAJE AÉREO DE TUBERÍA DE Ø 2-1/2”</t>
+        </is>
+      </c>
+      <c r="F1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1628" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="H1628" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX CSO/CSC MULTITAG ISSUE
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1628"/>
+  <dimension ref="A1:H1635"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
@@ -4802,7 +4802,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H225" t="inlineStr"/>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H238" t="inlineStr"/>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -9590,7 +9590,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H336" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H339" t="inlineStr"/>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H423" t="inlineStr"/>
@@ -17836,7 +17836,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H458" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H464" t="inlineStr"/>
@@ -18254,7 +18254,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H469" t="inlineStr"/>
@@ -18330,7 +18330,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H471" t="inlineStr"/>
@@ -20078,7 +20078,7 @@
       </c>
       <c r="G517" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>25,00</t>
         </is>
       </c>
       <c r="H517" t="inlineStr"/>
@@ -26500,7 +26500,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H686" t="inlineStr"/>
@@ -36114,7 +36114,7 @@
       </c>
       <c r="G939" t="inlineStr">
         <is>
-          <t>80,00</t>
+          <t>200,00</t>
         </is>
       </c>
       <c r="H939" t="inlineStr"/>
@@ -36418,7 +36418,7 @@
       </c>
       <c r="G947" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H947" t="inlineStr"/>
@@ -37862,7 +37862,7 @@
       </c>
       <c r="G985" t="inlineStr">
         <is>
-          <t>41,777</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H985" t="inlineStr"/>
@@ -37900,7 +37900,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>50,886</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H986" t="inlineStr"/>
@@ -37938,7 +37938,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>28,014</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H987" t="inlineStr"/>
@@ -37976,7 +37976,7 @@
       </c>
       <c r="G988" t="inlineStr">
         <is>
-          <t>146,561</t>
+          <t>60,85</t>
         </is>
       </c>
       <c r="H988" t="inlineStr"/>
@@ -38014,7 +38014,7 @@
       </c>
       <c r="G989" t="inlineStr">
         <is>
-          <t>821,582</t>
+          <t>337,956</t>
         </is>
       </c>
       <c r="H989" t="inlineStr"/>
@@ -38052,7 +38052,7 @@
       </c>
       <c r="G990" t="inlineStr">
         <is>
-          <t>116,204</t>
+          <t>555,298</t>
         </is>
       </c>
       <c r="H990" t="inlineStr"/>
@@ -39078,7 +39078,7 @@
       </c>
       <c r="G1017" t="inlineStr">
         <is>
-          <t>292,8</t>
+          <t>322,00</t>
         </is>
       </c>
       <c r="H1017" t="inlineStr"/>
@@ -39116,7 +39116,7 @@
       </c>
       <c r="G1018" t="inlineStr">
         <is>
-          <t>454,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1018" t="inlineStr"/>
@@ -39154,7 +39154,7 @@
       </c>
       <c r="G1019" t="inlineStr">
         <is>
-          <t>506,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1019" t="inlineStr"/>
@@ -39458,7 +39458,7 @@
       </c>
       <c r="G1027" t="inlineStr">
         <is>
-          <t>19,75</t>
+          <t>2,76</t>
         </is>
       </c>
       <c r="H1027" t="inlineStr"/>
@@ -39496,7 +39496,7 @@
       </c>
       <c r="G1028" t="inlineStr">
         <is>
-          <t>12,38</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1028" t="inlineStr"/>
@@ -39534,7 +39534,7 @@
       </c>
       <c r="G1029" t="inlineStr">
         <is>
-          <t>93,24</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1029" t="inlineStr"/>
@@ -39572,7 +39572,7 @@
       </c>
       <c r="G1030" t="inlineStr">
         <is>
-          <t>317,71</t>
+          <t>275,21</t>
         </is>
       </c>
       <c r="H1030" t="inlineStr"/>
@@ -39610,7 +39610,7 @@
       </c>
       <c r="G1031" t="inlineStr">
         <is>
-          <t>461,27</t>
+          <t>4212,77</t>
         </is>
       </c>
       <c r="H1031" t="inlineStr"/>
@@ -39648,7 +39648,7 @@
       </c>
       <c r="G1032" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>582,43</t>
         </is>
       </c>
       <c r="H1032" t="inlineStr"/>
@@ -39724,7 +39724,7 @@
       </c>
       <c r="G1034" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,5</t>
         </is>
       </c>
       <c r="H1034" t="inlineStr"/>
@@ -40522,7 +40522,7 @@
       </c>
       <c r="G1055" t="inlineStr">
         <is>
-          <t>19,75</t>
+          <t>2,76</t>
         </is>
       </c>
       <c r="H1055" t="inlineStr"/>
@@ -40560,7 +40560,7 @@
       </c>
       <c r="G1056" t="inlineStr">
         <is>
-          <t>12,38</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1056" t="inlineStr"/>
@@ -40598,7 +40598,7 @@
       </c>
       <c r="G1057" t="inlineStr">
         <is>
-          <t>93,24</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1057" t="inlineStr"/>
@@ -40636,7 +40636,7 @@
       </c>
       <c r="G1058" t="inlineStr">
         <is>
-          <t>317,71</t>
+          <t>275,21</t>
         </is>
       </c>
       <c r="H1058" t="inlineStr"/>
@@ -40674,7 +40674,7 @@
       </c>
       <c r="G1059" t="inlineStr">
         <is>
-          <t>461,27</t>
+          <t>4212,77</t>
         </is>
       </c>
       <c r="H1059" t="inlineStr"/>
@@ -40712,7 +40712,7 @@
       </c>
       <c r="G1060" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>582,43</t>
         </is>
       </c>
       <c r="H1060" t="inlineStr"/>
@@ -40788,7 +40788,7 @@
       </c>
       <c r="G1062" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,5</t>
         </is>
       </c>
       <c r="H1062" t="inlineStr"/>
@@ -42878,7 +42878,7 @@
       </c>
       <c r="G1117" t="inlineStr">
         <is>
-          <t>22,98</t>
+          <t>1,04</t>
         </is>
       </c>
       <c r="H1117" t="inlineStr"/>
@@ -42916,7 +42916,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>1,945</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>7,616</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>204,428</t>
+          <t>5,84</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>266,1</t>
+          <t>772,64</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43068,7 +43068,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>114,2</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -44018,7 +44018,7 @@
       </c>
       <c r="G1147" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1147" t="inlineStr"/>
@@ -44132,7 +44132,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr"/>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr"/>
@@ -44208,7 +44208,7 @@
       </c>
       <c r="G1152" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1152" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>15,84</t>
+          <t>164,01</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>15,84</t>
+          <t>164,01</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>15,84</t>
+          <t>164,01</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>15,84</t>
+          <t>164,01</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -47476,7 +47476,7 @@
       </c>
       <c r="G1238" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1238" t="inlineStr"/>
@@ -47514,7 +47514,7 @@
       </c>
       <c r="G1239" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1239" t="inlineStr"/>
@@ -47552,7 +47552,7 @@
       </c>
       <c r="G1240" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1240" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>548,4</t>
+          <t>181,44</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>34,8</t>
+          <t>15,6</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>120,225</t>
+          <t>983,325</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -57394,7 +57394,7 @@
       </c>
       <c r="G1499" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1499" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>47,74</t>
+          <t>180,33</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-30</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW FEMALE END ASME B16.11 SW 3000# FORGED ASTM A105, 1/2 "</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61316,7 +61316,7 @@
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>19,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -61348,17 +61348,17 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2-1/2 ", S-30</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -61390,17 +61390,17 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 4 ", S-30</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,17 +61432,17 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 6 ", S-40</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>127,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,17 +61474,17 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 8 ", S-20</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>13,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,7 +61516,7 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 6"</t>
+          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE 6"</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
@@ -61526,7 +61526,7 @@
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X120MMLG</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61568,7 +61568,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -61600,17 +61600,17 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3 ", S-40</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,17 +61642,17 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4 ", S-40</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, MSS SP-136, A536 Gr 65-45-12, CL 125, INST HORIZ/VERT, FF, B16.1, BOLTED COVER, NON METALLIC FLAT GASKET EPDM, SEATS BRONZE, DISC DUCTILE IRON EPDM ENCAPSULATED, SS304 PIN,UL LISTED/FM APPROVED, 6"</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>13,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,17 +61684,17 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6 ", S-40</t>
+          <t>SUMINISTRO DE TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,7 +61726,7 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
+          <t>SUMINISTRO DE CONC. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X4"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
@@ -61736,7 +61736,7 @@
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>32,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,7 +61768,7 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X125MMLG</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X6"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
@@ -61778,7 +61778,7 @@
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,7 +61810,7 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 4"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
@@ -61820,7 +61820,7 @@
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>84,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -61852,7 +61852,7 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 3"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 6"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
@@ -61862,7 +61862,7 @@
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -61894,7 +61894,7 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE LIFT CHECK VALVE SW, API 602, A105, CL 800, INST HORIZ/VERT, SW, B16.11, BOLTED COVER, SPW SS304/GRAPH, PISTON TYPE OBTURATOR, TRIM #8, 1/2"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 8"</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
@@ -61904,7 +61904,7 @@
       </c>
       <c r="G1616" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1616" t="inlineStr">
@@ -61936,7 +61936,7 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 4"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 6"</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
@@ -61946,7 +61946,7 @@
       </c>
       <c r="G1617" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1617" t="inlineStr">
@@ -61978,7 +61978,7 @@
       </c>
       <c r="E1618" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1/2"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 8"</t>
         </is>
       </c>
       <c r="F1618" t="inlineStr">
@@ -62020,7 +62020,7 @@
       </c>
       <c r="E1619" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE INTEGRAL MONO FLANGE DBB NEEDLE MULTI-VALVE, EEMUA 182, A105, CL 150, RF/NPTF, B16.5 AND B1.20.1, BB, SPW SS304/GRAPH, PKG GRAPH; SS316 STEM, SEATS&amp;STEM TIP, S, SWIVEL NEEDLE, STEM OS&amp;Y/RSRO, T-HANDLE, 3/4"</t>
+          <t>SUMINISTRO DE GATE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, S, SOLID WEDGE, STEM OS&amp;Y/RSNRO, HO, 1/2"</t>
         </is>
       </c>
       <c r="F1619" t="inlineStr">
@@ -62030,7 +62030,7 @@
       </c>
       <c r="G1619" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1619" t="inlineStr">
@@ -62062,7 +62062,7 @@
       </c>
       <c r="E1620" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4 ", S-80</t>
+          <t>SUMINISTRO DE ANGLE HOSE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREW-IN BONNET, RENEWABLE DISC, PKG NON ASBESTOS, DISC&amp;STEM BRONZE, RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
         </is>
       </c>
       <c r="F1620" t="inlineStr">
@@ -62072,7 +62072,7 @@
       </c>
       <c r="G1620" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1620" t="inlineStr">
@@ -62104,17 +62104,17 @@
       </c>
       <c r="E1621" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2 ", S-80</t>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1/2 ", S-XXS</t>
         </is>
       </c>
       <c r="F1621" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1621" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1621" t="inlineStr">
@@ -62146,17 +62146,17 @@
       </c>
       <c r="E1622" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4 ", S-80</t>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1½ ", S-160</t>
         </is>
       </c>
       <c r="F1622" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1622" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1622" t="inlineStr">
@@ -62188,7 +62188,7 @@
       </c>
       <c r="E1623" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3 " X 1/2 "</t>
+          <t>SUMINISTRO DE PIPExTE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 3/4 ", S-160</t>
         </is>
       </c>
       <c r="F1623" t="inlineStr">
@@ -62198,7 +62198,7 @@
       </c>
       <c r="G1623" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1623" t="inlineStr">
@@ -62230,7 +62230,7 @@
       </c>
       <c r="E1624" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4 " X 3/4 "</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 4"</t>
         </is>
       </c>
       <c r="F1624" t="inlineStr">
@@ -62272,7 +62272,7 @@
       </c>
       <c r="E1625" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 6 " X 3/4 "</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH20 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 4"</t>
         </is>
       </c>
       <c r="F1625" t="inlineStr">
@@ -62282,7 +62282,7 @@
       </c>
       <c r="G1625" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1625" t="inlineStr">
@@ -62314,7 +62314,7 @@
       </c>
       <c r="E1626" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 80, RF, ASTM A-105, ASME B16.5 2"</t>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 80 X SCH 80, PEXPE, ASTM A-234 GR WCB, MSS SP-95 1-1/2"X1"</t>
         </is>
       </c>
       <c r="F1626" t="inlineStr">
@@ -62324,7 +62324,7 @@
       </c>
       <c r="G1626" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1626" t="inlineStr">
@@ -62356,7 +62356,7 @@
       </c>
       <c r="E1627" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 80, RF, ASTM A-105, ASME B16.5 4"</t>
+          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 6 " X 1/2 "</t>
         </is>
       </c>
       <c r="F1627" t="inlineStr">
@@ -62398,20 +62398,314 @@
       </c>
       <c r="E1628" t="inlineStr">
         <is>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 4 ", S-30</t>
+        </is>
+      </c>
+      <c r="F1628" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1628" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1628" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1629" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 8 ", S-20</t>
+        </is>
+      </c>
+      <c r="F1629" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1629" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1629" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1630" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 6" X 2-1/2 ", S-40 X S-30</t>
+        </is>
+      </c>
+      <c r="F1630" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1630" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1630" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PREFABRICACIÓN EN TALLER DE TUBERÍA DE ACERO AL CARBÓN DE Ø 2-1/2" </t>
+        </is>
+      </c>
+      <c r="F1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1631" t="inlineStr">
+        <is>
+          <t>15,28</t>
+        </is>
+      </c>
+      <c r="H1631" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1632" t="inlineStr">
+        <is>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES BRIDADAS ANSI 150 DE DIAMETRO 2-1/2"</t>
+        </is>
+      </c>
+      <c r="F1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1632" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1632" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1633" t="inlineStr">
+        <is>
           <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
         </is>
       </c>
-      <c r="F1628" t="inlineStr">
+      <c r="F1633" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G1628" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1628" t="inlineStr">
+      <c r="G1633" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1633" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1634" t="inlineStr">
+        <is>
+          <t>MONTAJE AÉREO DE TUBERÍA DE Ø 2-1/2”</t>
+        </is>
+      </c>
+      <c r="F1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1634" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="H1634" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1635" t="inlineStr">
+        <is>
+          <t>MONTAJE DE VÁLVULAS Y CHEQUES DIAMETRO DE 2-1/2"</t>
+        </is>
+      </c>
+      <c r="F1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1635" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1635" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX FORGIVEN AND UNDERGROUND PIPING FOR DEMOLITION
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -37282,7 +37282,7 @@
       </c>
       <c r="E970" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø MENORES A 2" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø MENORES A 2" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F970" t="inlineStr">
@@ -37320,7 +37320,7 @@
       </c>
       <c r="E971" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 2" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 2" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F971" t="inlineStr">
@@ -37358,7 +37358,7 @@
       </c>
       <c r="E972" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 3" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 3" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F972" t="inlineStr">
@@ -37396,7 +37396,7 @@
       </c>
       <c r="E973" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 4" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 4" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F973" t="inlineStr">
@@ -37434,7 +37434,7 @@
       </c>
       <c r="E974" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 6" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 6" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F974" t="inlineStr">
@@ -37472,7 +37472,7 @@
       </c>
       <c r="E975" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 8" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 8" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F975" t="inlineStr">
@@ -37510,7 +37510,7 @@
       </c>
       <c r="E976" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 10" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 10" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F976" t="inlineStr">
@@ -37548,7 +37548,7 @@
       </c>
       <c r="E977" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 12" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 12" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F977" t="inlineStr">
@@ -37586,7 +37586,7 @@
       </c>
       <c r="E978" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 14" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 14" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F978" t="inlineStr">
@@ -37624,7 +37624,7 @@
       </c>
       <c r="E979" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 16" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 16" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F979" t="inlineStr">
@@ -37662,7 +37662,7 @@
       </c>
       <c r="E980" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 18" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 18" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F980" t="inlineStr">
@@ -37700,7 +37700,7 @@
       </c>
       <c r="E981" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 20" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 20" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F981" t="inlineStr">
@@ -37738,7 +37738,7 @@
       </c>
       <c r="E982" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 24" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 24" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F982" t="inlineStr">
@@ -37776,7 +37776,7 @@
       </c>
       <c r="E983" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 30" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 30" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F983" t="inlineStr">
@@ -37814,7 +37814,7 @@
       </c>
       <c r="E984" t="inlineStr">
         <is>
-          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADASDE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 36" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
+          <t>DESMANTELAMIENTO CON CORTE EN FRÍO DE TUBERÍAS ENTERRADAS DE ACERO AL CARBÓN, ACERO AL CARBON GALVANIZADO O ACERO INOXIDABLE Y ACCESORIOS DE Ø 36" (INCLUYE TRANSPORTE Y DISPOSICIÓN FINAL)</t>
         </is>
       </c>
       <c r="F984" t="inlineStr">
@@ -37976,7 +37976,7 @@
       </c>
       <c r="G988" t="inlineStr">
         <is>
-          <t>60,85</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H988" t="inlineStr"/>
@@ -38014,7 +38014,7 @@
       </c>
       <c r="G989" t="inlineStr">
         <is>
-          <t>337,956</t>
+          <t>95,26</t>
         </is>
       </c>
       <c r="H989" t="inlineStr"/>
@@ -38546,7 +38546,7 @@
       </c>
       <c r="G1003" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>60,85</t>
         </is>
       </c>
       <c r="H1003" t="inlineStr"/>
@@ -39344,7 +39344,7 @@
       </c>
       <c r="G1024" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,1958</t>
         </is>
       </c>
       <c r="H1024" t="inlineStr"/>

</xml_diff>

<commit_message>
UPDATE PIPING_CLASS PRE SOLVE FORGOTTEN PIPES
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1723"/>
+  <dimension ref="A1:H1670"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>23,00</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>19,00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H199" t="inlineStr"/>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>12,00</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -8640,7 +8640,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>41,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H216" t="inlineStr"/>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -9590,7 +9590,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -10274,7 +10274,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H259" t="inlineStr"/>
@@ -12250,7 +12250,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H311" t="inlineStr"/>
@@ -12288,7 +12288,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H312" t="inlineStr"/>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>27,00</t>
         </is>
       </c>
       <c r="H336" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>38,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>81,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H339" t="inlineStr"/>
@@ -13390,7 +13390,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>26,00</t>
         </is>
       </c>
       <c r="H341" t="inlineStr"/>
@@ -16430,7 +16430,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H421" t="inlineStr"/>
@@ -17912,7 +17912,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H460" t="inlineStr"/>
@@ -17950,7 +17950,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>25,00</t>
         </is>
       </c>
       <c r="H461" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>63,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>29,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>18,00</t>
         </is>
       </c>
       <c r="H464" t="inlineStr"/>
@@ -18102,7 +18102,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H465" t="inlineStr"/>
@@ -20078,7 +20078,7 @@
       </c>
       <c r="G517" t="inlineStr">
         <is>
-          <t>110,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H517" t="inlineStr"/>
@@ -20610,7 +20610,7 @@
       </c>
       <c r="G531" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H531" t="inlineStr"/>
@@ -26424,7 +26424,7 @@
       </c>
       <c r="G684" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H684" t="inlineStr"/>
@@ -36114,7 +36114,7 @@
       </c>
       <c r="G939" t="inlineStr">
         <is>
-          <t>1040,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H939" t="inlineStr"/>
@@ -36380,7 +36380,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H946" t="inlineStr"/>
@@ -36456,7 +36456,7 @@
       </c>
       <c r="G948" t="inlineStr">
         <is>
-          <t>336,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H948" t="inlineStr"/>
@@ -41662,7 +41662,7 @@
       </c>
       <c r="G1085" t="inlineStr">
         <is>
-          <t>136,73</t>
+          <t>30,748</t>
         </is>
       </c>
       <c r="H1085" t="inlineStr"/>
@@ -41700,7 +41700,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>729,988</t>
+          <t>242,865</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr"/>
@@ -41738,7 +41738,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>549,5</t>
+          <t>1156,874</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr"/>
@@ -41776,7 +41776,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>1580,54</t>
+          <t>3145,005</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr"/>
@@ -41814,7 +41814,7 @@
       </c>
       <c r="G1089" t="inlineStr">
         <is>
-          <t>13215,62</t>
+          <t>763,336</t>
         </is>
       </c>
       <c r="H1089" t="inlineStr"/>
@@ -41852,7 +41852,7 @@
       </c>
       <c r="G1090" t="inlineStr">
         <is>
-          <t>1628,56</t>
+          <t>1423,756</t>
         </is>
       </c>
       <c r="H1090" t="inlineStr"/>
@@ -41890,7 +41890,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>2471,392</t>
+          <t>9224,864</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr"/>
@@ -41928,7 +41928,7 @@
       </c>
       <c r="G1092" t="inlineStr">
         <is>
-          <t>15495,278</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1092" t="inlineStr"/>
@@ -41966,7 +41966,7 @@
       </c>
       <c r="G1093" t="inlineStr">
         <is>
-          <t>417,012</t>
+          <t>2143,774</t>
         </is>
       </c>
       <c r="H1093" t="inlineStr"/>
@@ -42004,7 +42004,7 @@
       </c>
       <c r="G1094" t="inlineStr">
         <is>
-          <t>2519,69</t>
+          <t>1379,894</t>
         </is>
       </c>
       <c r="H1094" t="inlineStr"/>
@@ -42422,7 +42422,7 @@
       </c>
       <c r="G1105" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>33,32</t>
         </is>
       </c>
       <c r="H1105" t="inlineStr"/>
@@ -42460,7 +42460,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>581,64</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr"/>
@@ -42878,7 +42878,7 @@
       </c>
       <c r="G1117" t="inlineStr">
         <is>
-          <t>80,89</t>
+          <t>36,6</t>
         </is>
       </c>
       <c r="H1117" t="inlineStr"/>
@@ -42916,7 +42916,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>305,9</t>
+          <t>82,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>203,00</t>
+          <t>475,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>308,00</t>
+          <t>225,00</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>1496,00</t>
+          <t>539,00</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43068,7 +43068,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>624,00</t>
+          <t>1152,00</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -43106,7 +43106,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>1264,00</t>
+          <t>2965,00</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr"/>
@@ -43144,7 +43144,7 @@
       </c>
       <c r="G1124" t="inlineStr">
         <is>
-          <t>3090,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1124" t="inlineStr"/>
@@ -43182,7 +43182,7 @@
       </c>
       <c r="G1125" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>406,00</t>
         </is>
       </c>
       <c r="H1125" t="inlineStr"/>
@@ -44056,7 +44056,7 @@
       </c>
       <c r="G1148" t="inlineStr">
         <is>
-          <t>49,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1148" t="inlineStr"/>
@@ -44094,7 +44094,7 @@
       </c>
       <c r="G1149" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>19,00</t>
         </is>
       </c>
       <c r="H1149" t="inlineStr"/>
@@ -44132,7 +44132,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr"/>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>22,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr"/>
@@ -44208,7 +44208,7 @@
       </c>
       <c r="G1152" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H1152" t="inlineStr"/>
@@ -44246,7 +44246,7 @@
       </c>
       <c r="G1153" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1153" t="inlineStr"/>
@@ -44284,7 +44284,7 @@
       </c>
       <c r="G1154" t="inlineStr">
         <is>
-          <t>13,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1154" t="inlineStr"/>
@@ -44322,7 +44322,7 @@
       </c>
       <c r="G1155" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1155" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>251,91</t>
+          <t>359,3</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>251,91</t>
+          <t>359,3</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>251,91</t>
+          <t>359,3</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>251,91</t>
+          <t>359,3</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>1541,52</t>
+          <t>5049,6</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>187,5</t>
+          <t>71,4</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>6828,9375</t>
+          <t>3168,375</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -57356,7 +57356,7 @@
       </c>
       <c r="G1498" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1498" t="inlineStr"/>
@@ -57432,7 +57432,7 @@
       </c>
       <c r="G1500" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1500" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>1406,97</t>
+          <t>799,04</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 3"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 2"</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61316,7 +61316,7 @@
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -61348,7 +61348,7 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW FEMALE END ASME B16.11 SW 6000# FORGED ASTM A105, 1/2"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
@@ -61358,7 +61358,7 @@
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -61390,7 +61390,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-20</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-30</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -61400,7 +61400,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>20,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,7 +61432,7 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 12", S-20</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-30</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
@@ -61442,7 +61442,7 @@
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>32,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,7 +61474,7 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-STD</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 2", S-40</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
@@ -61484,7 +61484,7 @@
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,7 +61516,7 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 16", S-STD</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
@@ -61526,7 +61526,7 @@
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>28,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 2", S-40</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61568,7 +61568,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>34,00</t>
+          <t>21,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -61600,7 +61600,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -61610,7 +61610,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>15,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,7 +61642,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-30</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -61652,7 +61652,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,7 +61684,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 3"</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -61694,7 +61694,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>84,00</t>
+          <t>19,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,17 +61726,17 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>55,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,17 +61768,17 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 10", S-20</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 6"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>27,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,17 +61810,17 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 12", S-20</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>231,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -61852,12 +61852,12 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 14", S-STD</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1615" t="inlineStr">
@@ -61894,17 +61894,17 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 16", S-STD</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1616" t="inlineStr">
         <is>
-          <t>15,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1616" t="inlineStr">
@@ -61936,7 +61936,7 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2", S-80</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 10", S-30</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
@@ -61946,7 +61946,7 @@
       </c>
       <c r="G1617" t="inlineStr">
         <is>
-          <t>35,00</t>
+          <t>143,00</t>
         </is>
       </c>
       <c r="H1617" t="inlineStr">
@@ -61978,7 +61978,7 @@
       </c>
       <c r="E1618" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2-1/2", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 14", S-30</t>
         </is>
       </c>
       <c r="F1618" t="inlineStr">
@@ -61988,7 +61988,7 @@
       </c>
       <c r="G1618" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>23,00</t>
         </is>
       </c>
       <c r="H1618" t="inlineStr">
@@ -62020,7 +62020,7 @@
       </c>
       <c r="E1619" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 3", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 18", S-40</t>
         </is>
       </c>
       <c r="F1619" t="inlineStr">
@@ -62030,7 +62030,7 @@
       </c>
       <c r="G1619" t="inlineStr">
         <is>
-          <t>42,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1619" t="inlineStr">
@@ -62062,7 +62062,7 @@
       </c>
       <c r="E1620" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 4", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
         </is>
       </c>
       <c r="F1620" t="inlineStr">
@@ -62072,7 +62072,7 @@
       </c>
       <c r="G1620" t="inlineStr">
         <is>
-          <t>80,00</t>
+          <t>25,00</t>
         </is>
       </c>
       <c r="H1620" t="inlineStr">
@@ -62104,7 +62104,7 @@
       </c>
       <c r="E1621" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 6", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
         </is>
       </c>
       <c r="F1621" t="inlineStr">
@@ -62114,7 +62114,7 @@
       </c>
       <c r="G1621" t="inlineStr">
         <is>
-          <t>375,00</t>
+          <t>76,00</t>
         </is>
       </c>
       <c r="H1621" t="inlineStr">
@@ -62146,7 +62146,7 @@
       </c>
       <c r="E1622" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 8", S-20</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
         </is>
       </c>
       <c r="F1622" t="inlineStr">
@@ -62156,7 +62156,7 @@
       </c>
       <c r="G1622" t="inlineStr">
         <is>
-          <t>38,00</t>
+          <t>147,00</t>
         </is>
       </c>
       <c r="H1622" t="inlineStr">
@@ -62188,17 +62188,17 @@
       </c>
       <c r="E1623" t="inlineStr">
         <is>
-          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE 10"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6", S-40</t>
         </is>
       </c>
       <c r="F1623" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1623" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1623" t="inlineStr">
@@ -62230,7 +62230,7 @@
       </c>
       <c r="E1624" t="inlineStr">
         <is>
-          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE 12"</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 1-1/2"</t>
         </is>
       </c>
       <c r="F1624" t="inlineStr">
@@ -62240,7 +62240,7 @@
       </c>
       <c r="G1624" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1624" t="inlineStr">
@@ -62272,7 +62272,7 @@
       </c>
       <c r="E1625" t="inlineStr">
         <is>
-          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE 6"</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 10"</t>
         </is>
       </c>
       <c r="F1625" t="inlineStr">
@@ -62282,7 +62282,7 @@
       </c>
       <c r="G1625" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1625" t="inlineStr">
@@ -62314,7 +62314,7 @@
       </c>
       <c r="E1626" t="inlineStr">
         <is>
-          <t>SUMINISTRO BLIND FLANGE, CLASS 150, FF, ASTM A105, ASME B16.5. DIAMETRO DE, 16"</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 16"</t>
         </is>
       </c>
       <c r="F1626" t="inlineStr">
@@ -62356,7 +62356,7 @@
       </c>
       <c r="E1627" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X145MMLG</t>
+          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 2"</t>
         </is>
       </c>
       <c r="F1627" t="inlineStr">
@@ -62366,7 +62366,7 @@
       </c>
       <c r="G1627" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1627" t="inlineStr">
@@ -62398,7 +62398,7 @@
       </c>
       <c r="E1628" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X150MMLG</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
         </is>
       </c>
       <c r="F1628" t="inlineStr">
@@ -62408,7 +62408,7 @@
       </c>
       <c r="G1628" t="inlineStr">
         <is>
-          <t>32,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1628" t="inlineStr">
@@ -62440,7 +62440,7 @@
       </c>
       <c r="E1629" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X120MMLG</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 2"</t>
         </is>
       </c>
       <c r="F1629" t="inlineStr">
@@ -62450,7 +62450,7 @@
       </c>
       <c r="G1629" t="inlineStr">
         <is>
-          <t>128,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1629" t="inlineStr">
@@ -62482,7 +62482,7 @@
       </c>
       <c r="E1630" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1-1/2"</t>
         </is>
       </c>
       <c r="F1630" t="inlineStr">
@@ -62492,7 +62492,7 @@
       </c>
       <c r="G1630" t="inlineStr">
         <is>
-          <t>460,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1630" t="inlineStr">
@@ -62524,7 +62524,7 @@
       </c>
       <c r="E1631" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø7/8"X135MMLG</t>
+          <t>SUMINISTRO DE CONC. REDUCER, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X8"</t>
         </is>
       </c>
       <c r="F1631" t="inlineStr">
@@ -62534,7 +62534,7 @@
       </c>
       <c r="G1631" t="inlineStr">
         <is>
-          <t>444,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1631" t="inlineStr">
@@ -62566,7 +62566,7 @@
       </c>
       <c r="E1632" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, MSS SP-136, A536 Gr 65-45-12, CL 125, INST HORIZ/VERT, FF, B16.1, BOLTED COVER, NON METALLIC FLAT GASKET EPDM, SEATS BRONZE, DISC DUCTILE IRON EPDM ENCAPSULATED, SS304 PIN,UL LISTED/FM APPROVED, 12"</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X8"</t>
         </is>
       </c>
       <c r="F1632" t="inlineStr">
@@ -62608,7 +62608,7 @@
       </c>
       <c r="E1633" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, MSS SP-136, A536 Gr 65-45-12, CL 125, INST HORIZ/VERT, FF, B16.1, BOLTED COVER, NON METALLIC FLAT GASKET EPDM, SEATS BRONZE, DISC DUCTILE IRON EPDM ENCAPSULATED, SS304 PIN,UL LISTED/FM APPROVED, 2"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 10"</t>
         </is>
       </c>
       <c r="F1633" t="inlineStr">
@@ -62618,7 +62618,7 @@
       </c>
       <c r="G1633" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>38,00</t>
         </is>
       </c>
       <c r="H1633" t="inlineStr">
@@ -62650,7 +62650,7 @@
       </c>
       <c r="E1634" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X10"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 14"</t>
         </is>
       </c>
       <c r="F1634" t="inlineStr">
@@ -62660,7 +62660,7 @@
       </c>
       <c r="G1634" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1634" t="inlineStr">
@@ -62692,7 +62692,7 @@
       </c>
       <c r="E1635" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X8"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 16"</t>
         </is>
       </c>
       <c r="F1635" t="inlineStr">
@@ -62734,7 +62734,7 @@
       </c>
       <c r="E1636" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 4"X3"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 14"</t>
         </is>
       </c>
       <c r="F1636" t="inlineStr">
@@ -62776,7 +62776,7 @@
       </c>
       <c r="E1637" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X3"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 10"</t>
         </is>
       </c>
       <c r="F1637" t="inlineStr">
@@ -62786,7 +62786,7 @@
       </c>
       <c r="G1637" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H1637" t="inlineStr">
@@ -62818,7 +62818,7 @@
       </c>
       <c r="E1638" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X4"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 2"</t>
         </is>
       </c>
       <c r="F1638" t="inlineStr">
@@ -62860,7 +62860,7 @@
       </c>
       <c r="E1639" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 14"X8"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 8"</t>
         </is>
       </c>
       <c r="F1639" t="inlineStr">
@@ -62870,7 +62870,7 @@
       </c>
       <c r="G1639" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H1639" t="inlineStr">
@@ -62902,7 +62902,7 @@
       </c>
       <c r="E1640" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 16"X12"</t>
+          <t>SUMINISTRO DE GLOBE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PLUG DISC, STEM OS&amp;Y/RSRO, HO, 1/2"</t>
         </is>
       </c>
       <c r="F1640" t="inlineStr">
@@ -62912,7 +62912,7 @@
       </c>
       <c r="G1640" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1640" t="inlineStr">
@@ -62944,7 +62944,7 @@
       </c>
       <c r="E1641" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 10"</t>
+          <t>SUMINISTRO DE GLOBE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PLUG DISC, STEM OS&amp;Y/RSRO, HO, 3/4"</t>
         </is>
       </c>
       <c r="F1641" t="inlineStr">
@@ -62954,7 +62954,7 @@
       </c>
       <c r="G1641" t="inlineStr">
         <is>
-          <t>29,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1641" t="inlineStr">
@@ -62986,7 +62986,7 @@
       </c>
       <c r="E1642" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 12"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1/2", S-80</t>
         </is>
       </c>
       <c r="F1642" t="inlineStr">
@@ -62996,7 +62996,7 @@
       </c>
       <c r="G1642" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1642" t="inlineStr">
@@ -63028,7 +63028,7 @@
       </c>
       <c r="E1643" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 14"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1643" t="inlineStr">
@@ -63038,7 +63038,7 @@
       </c>
       <c r="G1643" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1643" t="inlineStr">
@@ -63070,17 +63070,17 @@
       </c>
       <c r="E1644" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 16"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
         </is>
       </c>
       <c r="F1644" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1644" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1644" t="inlineStr">
@@ -63112,17 +63112,17 @@
       </c>
       <c r="E1645" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 2"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1-1/2", S-80</t>
         </is>
       </c>
       <c r="F1645" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1645" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1645" t="inlineStr">
@@ -63154,17 +63154,17 @@
       </c>
       <c r="E1646" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 3"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
         </is>
       </c>
       <c r="F1646" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1646" t="inlineStr">
         <is>
-          <t>27,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1646" t="inlineStr">
@@ -63196,17 +63196,17 @@
       </c>
       <c r="E1647" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 4"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1647" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1647" t="inlineStr">
         <is>
-          <t>51,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1647" t="inlineStr">
@@ -63238,7 +63238,7 @@
       </c>
       <c r="E1648" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 6"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X 8"</t>
         </is>
       </c>
       <c r="F1648" t="inlineStr">
@@ -63248,7 +63248,7 @@
       </c>
       <c r="G1648" t="inlineStr">
         <is>
-          <t>122,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1648" t="inlineStr">
@@ -63280,7 +63280,7 @@
       </c>
       <c r="E1649" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 8"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 10"X 6"</t>
         </is>
       </c>
       <c r="F1649" t="inlineStr">
@@ -63290,7 +63290,7 @@
       </c>
       <c r="G1649" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1649" t="inlineStr">
@@ -63322,7 +63322,7 @@
       </c>
       <c r="E1650" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 10"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 10"</t>
         </is>
       </c>
       <c r="F1650" t="inlineStr">
@@ -63332,7 +63332,7 @@
       </c>
       <c r="G1650" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1650" t="inlineStr">
@@ -63364,7 +63364,7 @@
       </c>
       <c r="E1651" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 12"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 14"</t>
         </is>
       </c>
       <c r="F1651" t="inlineStr">
@@ -63374,7 +63374,7 @@
       </c>
       <c r="G1651" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1651" t="inlineStr">
@@ -63406,7 +63406,7 @@
       </c>
       <c r="E1652" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 1"</t>
         </is>
       </c>
       <c r="F1652" t="inlineStr">
@@ -63416,7 +63416,7 @@
       </c>
       <c r="G1652" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1652" t="inlineStr">
@@ -63448,7 +63448,7 @@
       </c>
       <c r="E1653" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 3"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 1-1/2"</t>
         </is>
       </c>
       <c r="F1653" t="inlineStr">
@@ -63458,7 +63458,7 @@
       </c>
       <c r="G1653" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1653" t="inlineStr">
@@ -63490,7 +63490,7 @@
       </c>
       <c r="E1654" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 4"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 3/4"</t>
         </is>
       </c>
       <c r="F1654" t="inlineStr">
@@ -63500,7 +63500,7 @@
       </c>
       <c r="G1654" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1654" t="inlineStr">
@@ -63532,7 +63532,7 @@
       </c>
       <c r="E1655" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 6"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 16" X 3/4"</t>
         </is>
       </c>
       <c r="F1655" t="inlineStr">
@@ -63542,7 +63542,7 @@
       </c>
       <c r="G1655" t="inlineStr">
         <is>
-          <t>22,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1655" t="inlineStr">
@@ -63574,7 +63574,7 @@
       </c>
       <c r="E1656" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 8"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 2" X 1/2"</t>
         </is>
       </c>
       <c r="F1656" t="inlineStr">
@@ -63584,7 +63584,7 @@
       </c>
       <c r="G1656" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1656" t="inlineStr">
@@ -63616,7 +63616,7 @@
       </c>
       <c r="E1657" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, S, SOLID WEDGE, STEM OS&amp;Y/RSNRO, HO, 1"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 3/4"</t>
         </is>
       </c>
       <c r="F1657" t="inlineStr">
@@ -63626,7 +63626,7 @@
       </c>
       <c r="G1657" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1657" t="inlineStr">
@@ -63658,7 +63658,7 @@
       </c>
       <c r="E1658" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, S, SOLID WEDGE, STEM OS&amp;Y/RSNRO, HO, 1/2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 8" X 3/4"</t>
         </is>
       </c>
       <c r="F1658" t="inlineStr">
@@ -63668,7 +63668,7 @@
       </c>
       <c r="G1658" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1658" t="inlineStr">
@@ -63700,7 +63700,7 @@
       </c>
       <c r="E1659" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ANGLE HOSE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREW-IN BONNET, RENEWABLE DISC, PKG NON ASBESTOS, DISC&amp;STEM BRONZE, RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
+          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
         </is>
       </c>
       <c r="F1659" t="inlineStr">
@@ -63710,7 +63710,7 @@
       </c>
       <c r="G1659" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1659" t="inlineStr">
@@ -63742,7 +63742,7 @@
       </c>
       <c r="E1660" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GLOBE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, SWIVEL PLUG DISC, STEM IS/RSRO, HO, UL LISTED, 1-1/2"</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 10"</t>
         </is>
       </c>
       <c r="F1660" t="inlineStr">
@@ -63752,7 +63752,7 @@
       </c>
       <c r="G1660" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>46,00</t>
         </is>
       </c>
       <c r="H1660" t="inlineStr">
@@ -63784,7 +63784,7 @@
       </c>
       <c r="E1661" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GLOBE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, SWIVEL PLUG DISC, STEM IS/RSRO, HO, UL LISTED, 2"</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 14"</t>
         </is>
       </c>
       <c r="F1661" t="inlineStr">
@@ -63794,7 +63794,7 @@
       </c>
       <c r="G1661" t="inlineStr">
         <is>
-          <t>47,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1661" t="inlineStr">
@@ -63826,7 +63826,7 @@
       </c>
       <c r="E1662" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GLOBE VALVE THD, MSS SP-80, B62 UNS C83600, CL 150, NPTF, B1.20.1, SCREWED BONNET, PKG LUBRICATED FIBER/GRAPH, BRONZE STEM, SEAT RINGS&amp;DISC, SWIVEL PLUG DISC, STEM IS/RSRO, HO, UL LISTED, 3/4"</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 40, RF, ASTM A-105, ASME B16.5 16"</t>
         </is>
       </c>
       <c r="F1662" t="inlineStr">
@@ -63836,7 +63836,7 @@
       </c>
       <c r="G1662" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1662" t="inlineStr">
@@ -63868,7 +63868,7 @@
       </c>
       <c r="E1663" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 BExTE SEAMLESS ASTM A53 GR. B, 2", S-160</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 10" X 2", S-30 X S-40</t>
         </is>
       </c>
       <c r="F1663" t="inlineStr">
@@ -63878,7 +63878,7 @@
       </c>
       <c r="G1663" t="inlineStr">
         <is>
-          <t>70,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H1663" t="inlineStr">
@@ -63910,7 +63910,7 @@
       </c>
       <c r="E1664" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A53 GR. B, 1", S-160</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 10" X 3", S-30 X S-40</t>
         </is>
       </c>
       <c r="F1664" t="inlineStr">
@@ -63952,7 +63952,7 @@
       </c>
       <c r="E1665" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A53 GR. B, 3/4", S-160</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 8" X 2", S-20 X S-40</t>
         </is>
       </c>
       <c r="F1665" t="inlineStr">
@@ -63962,7 +63962,7 @@
       </c>
       <c r="G1665" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1665" t="inlineStr">
@@ -63994,17 +63994,17 @@
       </c>
       <c r="E1666" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1", S-160</t>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
         </is>
       </c>
       <c r="F1666" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1666" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1666" t="inlineStr">
@@ -64036,17 +64036,17 @@
       </c>
       <c r="E1667" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PExTE SEAMLESS ASTM A53 GR. B, 1-1/2", S-160</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1667" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1667" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>8,92</t>
         </is>
       </c>
       <c r="H1667" t="inlineStr">
@@ -64078,17 +64078,17 @@
       </c>
       <c r="E1668" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 TE SEAMLESS ASTM A53 GR. B, 1-1/2", S-160</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1668" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1668" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>36,00</t>
         </is>
       </c>
       <c r="H1668" t="inlineStr">
@@ -64120,17 +64120,17 @@
       </c>
       <c r="E1669" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 TE SEAMLESS ASTM A53 GR. B, 1/2", S-XXS</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1669" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1669" t="inlineStr">
         <is>
-          <t>72,00</t>
+          <t>23,00</t>
         </is>
       </c>
       <c r="H1669" t="inlineStr">
@@ -64162,2246 +64162,20 @@
       </c>
       <c r="E1670" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 TE SEAMLESS ASTM A53 GR. B, 3/4", S-160</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1670" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1670" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1670" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1671">
-      <c r="A1671" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1671" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1671" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1671" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1671" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 1", S-80</t>
-        </is>
-      </c>
-      <c r="F1671" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1671" t="inlineStr">
-        <is>
-          <t>10,00</t>
-        </is>
-      </c>
-      <c r="H1671" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1672">
-      <c r="A1672" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1672" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1672" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1672" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1672" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 1-1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1672" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1672" t="inlineStr">
-        <is>
-          <t>6,00</t>
-        </is>
-      </c>
-      <c r="H1672" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1673">
-      <c r="A1673" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1673" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1673" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1673" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1673" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 1/2", S-160</t>
-        </is>
-      </c>
-      <c r="F1673" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1673" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1673" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1674">
-      <c r="A1674" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1674" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1674" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1674" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1674" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 3/4", S-80</t>
-        </is>
-      </c>
-      <c r="F1674" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1674" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1674" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1675">
-      <c r="A1675" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1675" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1675" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1675" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1675" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 10"X 6"</t>
-        </is>
-      </c>
-      <c r="F1675" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1675" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="H1675" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1676">
-      <c r="A1676" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1676" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1676" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1676" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1676" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X 10"</t>
-        </is>
-      </c>
-      <c r="F1676" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1676" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1676" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1677">
-      <c r="A1677" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1677" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1677" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1677" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1677" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X 8"</t>
-        </is>
-      </c>
-      <c r="F1677" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1677" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1677" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1678">
-      <c r="A1678" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1678" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1678" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1678" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1678" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 80, BW, ASTM A-234 GR WPB, ASME B16.9 4"X 2"</t>
-        </is>
-      </c>
-      <c r="F1678" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1678" t="inlineStr">
-        <is>
-          <t>14,00</t>
-        </is>
-      </c>
-      <c r="H1678" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1679">
-      <c r="A1679" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1679" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1679" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1679" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1679" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 3"</t>
-        </is>
-      </c>
-      <c r="F1679" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1679" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1679" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1680">
-      <c r="A1680" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1680" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1680" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1680" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1680" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 4"</t>
-        </is>
-      </c>
-      <c r="F1680" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1680" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1680" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1681">
-      <c r="A1681" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1681" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1681" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1681" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1681" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 10"</t>
-        </is>
-      </c>
-      <c r="F1681" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1681" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1681" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1682">
-      <c r="A1682" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1682" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1682" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1682" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1682" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 12"</t>
-        </is>
-      </c>
-      <c r="F1682" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1682" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1682" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1683">
-      <c r="A1683" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1683" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1683" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1683" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1683" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 14"</t>
-        </is>
-      </c>
-      <c r="F1683" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1683" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1683" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1684">
-      <c r="A1684" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1684" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1684" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1684" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1684" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1684" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1684" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1684" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1685">
-      <c r="A1685" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1685" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1685" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1685" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1685" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE CONC. SWAGE, SCH 80 X SCH 80, PEXPE, ASTM A-234 GR WCB, MSS SP-95 1"X1/2"</t>
-        </is>
-      </c>
-      <c r="F1685" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1685" t="inlineStr">
-        <is>
-          <t>7,00</t>
-        </is>
-      </c>
-      <c r="H1685" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1686">
-      <c r="A1686" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1686" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1686" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1686" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1686" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"</t>
-        </is>
-      </c>
-      <c r="F1686" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1686" t="inlineStr">
-        <is>
-          <t>10,00</t>
-        </is>
-      </c>
-      <c r="H1686" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1687">
-      <c r="A1687" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1687" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1687" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1687" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1687" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 3"</t>
-        </is>
-      </c>
-      <c r="F1687" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1687" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1687" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1688">
-      <c r="A1688" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1688" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1688" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1688" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1688" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
-        </is>
-      </c>
-      <c r="F1688" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1688" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1688" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1689">
-      <c r="A1689" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1689" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1689" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1689" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1689" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"</t>
-        </is>
-      </c>
-      <c r="F1689" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1689" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1689" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1690">
-      <c r="A1690" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1690" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1690" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1690" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1690" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12" X 1"</t>
-        </is>
-      </c>
-      <c r="F1690" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1690" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1690" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1691">
-      <c r="A1691" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1691" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1691" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1691" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1691" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1691" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1691" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1691" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1692">
-      <c r="A1692" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1692" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1692" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1692" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1692" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 16" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1692" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1692" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1692" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1693">
-      <c r="A1693" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1693" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1693" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1693" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1693" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 1-1/2"</t>
-        </is>
-      </c>
-      <c r="F1693" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1693" t="inlineStr">
-        <is>
-          <t>6,00</t>
-        </is>
-      </c>
-      <c r="H1693" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1694">
-      <c r="A1694" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1694" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1694" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1694" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1694" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 6" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1694" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1694" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1694" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1695">
-      <c r="A1695" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1695" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1695" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1695" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1695" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 12" X 1/2"</t>
-        </is>
-      </c>
-      <c r="F1695" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1695" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1695" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1696">
-      <c r="A1696" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1696" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1696" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1696" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1696" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 16" X 1/2"</t>
-        </is>
-      </c>
-      <c r="F1696" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1696" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1696" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1697">
-      <c r="A1697" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1697" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1697" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1697" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1697" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 2" X 1/2"</t>
-        </is>
-      </c>
-      <c r="F1697" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1697" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1697" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1698">
-      <c r="A1698" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1698" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1698" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1698" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1698" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE THREADOLET MSS SP-97 BW X SW 6000# FORGED ASTM A105, 6" X 1/2"</t>
-        </is>
-      </c>
-      <c r="F1698" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1698" t="inlineStr">
-        <is>
-          <t>34,00</t>
-        </is>
-      </c>
-      <c r="H1698" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1699">
-      <c r="A1699" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1699" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1699" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1699" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1699" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE UNION, CS, ASTM A105, MSS SP-83, THD, CLASS 3000, 1-1/2"</t>
-        </is>
-      </c>
-      <c r="F1699" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1699" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1699" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1700">
-      <c r="A1700" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1700" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1700" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1700" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1700" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE UNION, CS, ASTM A105, MSS SP-83, THD, CLASS 3000, 3/4"</t>
-        </is>
-      </c>
-      <c r="F1700" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1700" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1700" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1701">
-      <c r="A1701" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1701" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1701" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1701" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1701" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 10", S-20</t>
-        </is>
-      </c>
-      <c r="F1701" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1701" t="inlineStr">
-        <is>
-          <t>24,00</t>
-        </is>
-      </c>
-      <c r="H1701" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1702">
-      <c r="A1702" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1702" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1702" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1702" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1702" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 12", S-20</t>
-        </is>
-      </c>
-      <c r="F1702" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1702" t="inlineStr">
-        <is>
-          <t>31,00</t>
-        </is>
-      </c>
-      <c r="H1702" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1703">
-      <c r="A1703" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1703" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1703" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1703" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1703" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 14", S-STD</t>
-        </is>
-      </c>
-      <c r="F1703" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1703" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1703" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1704">
-      <c r="A1704" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1704" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1704" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1704" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1704" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 16", S-STD</t>
-        </is>
-      </c>
-      <c r="F1704" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1704" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1704" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1705">
-      <c r="A1705" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1705" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1705" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1705" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1705" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 3", S-30</t>
-        </is>
-      </c>
-      <c r="F1705" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1705" t="inlineStr">
-        <is>
-          <t>17,00</t>
-        </is>
-      </c>
-      <c r="H1705" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1706">
-      <c r="A1706" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1706" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1706" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1706" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1706" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 4", S-30</t>
-        </is>
-      </c>
-      <c r="F1706" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1706" t="inlineStr">
-        <is>
-          <t>41,00</t>
-        </is>
-      </c>
-      <c r="H1706" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1707">
-      <c r="A1707" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1707" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1707" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1707" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1707" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 8", S-20</t>
-        </is>
-      </c>
-      <c r="F1707" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1707" t="inlineStr">
-        <is>
-          <t>14,00</t>
-        </is>
-      </c>
-      <c r="H1707" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1708">
-      <c r="A1708" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1708" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1708" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1708" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1708" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 10" X 2", S-20 X S-80</t>
-        </is>
-      </c>
-      <c r="F1708" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1708" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1708" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1709">
-      <c r="A1709" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1709" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1709" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1709" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1709" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 12" X 2", S-20 X S-80</t>
-        </is>
-      </c>
-      <c r="F1709" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1709" t="inlineStr">
-        <is>
-          <t>7,00</t>
-        </is>
-      </c>
-      <c r="H1709" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1710">
-      <c r="A1710" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1710" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1710" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1710" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1710" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 12" X 2-1/2", S-STD X S-30</t>
-        </is>
-      </c>
-      <c r="F1710" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1710" t="inlineStr">
-        <is>
-          <t>8,00</t>
-        </is>
-      </c>
-      <c r="H1710" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1711">
-      <c r="A1711" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1711" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1711" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1711" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1711" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 12" X 3", S-20 X S-30</t>
-        </is>
-      </c>
-      <c r="F1711" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1711" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1711" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1712">
-      <c r="A1712" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1712" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1712" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1712" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1712" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 16" X 2", S-STD X S-80</t>
-        </is>
-      </c>
-      <c r="F1712" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1712" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1712" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1713">
-      <c r="A1713" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1713" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1713" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1713" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1713" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 6" X 2", S-40 X S-80</t>
-        </is>
-      </c>
-      <c r="F1713" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1713" t="inlineStr">
-        <is>
-          <t>23,00</t>
-        </is>
-      </c>
-      <c r="H1713" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1714">
-      <c r="A1714" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1714" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1714" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1714" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1714" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 8" X 2", S-20 X S-80</t>
-        </is>
-      </c>
-      <c r="F1714" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1714" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1714" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1715">
-      <c r="A1715" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1715" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1715" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1715" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1715" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SUMINISTRO DE FILTROS TIPO Y ANSI 150 DE Ø 12" </t>
-        </is>
-      </c>
-      <c r="F1715" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1715" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1715" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1716">
-      <c r="A1716" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1716" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1716" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1716" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1716" t="inlineStr">
-        <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES BRIDADAS ANSI 150 DE DIAMETRO 2-1/2"</t>
-        </is>
-      </c>
-      <c r="F1716" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1716" t="inlineStr">
-        <is>
-          <t>8,00</t>
-        </is>
-      </c>
-      <c r="H1716" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1717">
-      <c r="A1717" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1717" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1717" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1717" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1717" t="inlineStr">
-        <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
-        </is>
-      </c>
-      <c r="F1717" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1717" t="inlineStr">
-        <is>
-          <t>55,00</t>
-        </is>
-      </c>
-      <c r="H1717" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1718">
-      <c r="A1718" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1718" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1718" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1718" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1718" t="inlineStr">
-        <is>
-          <t>MONTAJE AÉREO DE TUBERÍA DE Ø 2-1/2" (SIN PREFABRICAR)</t>
-        </is>
-      </c>
-      <c r="F1718" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1718" t="inlineStr">
-        <is>
-          <t>10,00</t>
-        </is>
-      </c>
-      <c r="H1718" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1719">
-      <c r="A1719" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1719" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1719" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1719" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1719" t="inlineStr">
-        <is>
-          <t>MONTAJE DE VÁLVULAS Y CHEQUES DIAMETRO DE 2-1/2"</t>
-        </is>
-      </c>
-      <c r="F1719" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1719" t="inlineStr">
-        <is>
-          <t>8,00</t>
-        </is>
-      </c>
-      <c r="H1719" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1720">
-      <c r="A1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F1720" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1720" t="inlineStr">
-        <is>
-          <t>8,92</t>
-        </is>
-      </c>
-      <c r="H1720" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1721">
-      <c r="A1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F1721" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1721" t="inlineStr">
-        <is>
-          <t>93,00</t>
-        </is>
-      </c>
-      <c r="H1721" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1722">
-      <c r="A1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F1722" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1722" t="inlineStr">
-        <is>
-          <t>27,00</t>
-        </is>
-      </c>
-      <c r="H1722" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1723">
-      <c r="A1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F1723" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1723" t="inlineStr">
-        <is>
-          <t>55,00</t>
-        </is>
-      </c>
-      <c r="H1723" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX FORGIVEN AND UNDERGROUND PIPE FOR DEMOLITION
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1670"/>
+  <dimension ref="A1:H1669"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37862,7 +37862,7 @@
       </c>
       <c r="G985" t="inlineStr">
         <is>
-          <t>113,162</t>
+          <t>30,748</t>
         </is>
       </c>
       <c r="H985" t="inlineStr"/>
@@ -37900,7 +37900,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>205,602</t>
+          <t>242,865</t>
         </is>
       </c>
       <c r="H986" t="inlineStr"/>
@@ -37938,7 +37938,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>348,74</t>
+          <t>819,694</t>
         </is>
       </c>
       <c r="H987" t="inlineStr"/>
@@ -37976,7 +37976,7 @@
       </c>
       <c r="G988" t="inlineStr">
         <is>
-          <t>519,23</t>
+          <t>2758,325</t>
         </is>
       </c>
       <c r="H988" t="inlineStr"/>
@@ -38014,7 +38014,7 @@
       </c>
       <c r="G989" t="inlineStr">
         <is>
-          <t>2559,858</t>
+          <t>1131,336</t>
         </is>
       </c>
       <c r="H989" t="inlineStr"/>
@@ -38052,7 +38052,7 @@
       </c>
       <c r="G990" t="inlineStr">
         <is>
-          <t>1666,372</t>
+          <t>1423,756</t>
         </is>
       </c>
       <c r="H990" t="inlineStr"/>
@@ -38090,7 +38090,7 @@
       </c>
       <c r="G991" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5497,664</t>
         </is>
       </c>
       <c r="H991" t="inlineStr"/>
@@ -38166,7 +38166,7 @@
       </c>
       <c r="G993" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2143,774</t>
         </is>
       </c>
       <c r="H993" t="inlineStr"/>
@@ -38204,7 +38204,7 @@
       </c>
       <c r="G994" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1379,894</t>
         </is>
       </c>
       <c r="H994" t="inlineStr"/>
@@ -38622,7 +38622,7 @@
       </c>
       <c r="G1005" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>33,32</t>
         </is>
       </c>
       <c r="H1005" t="inlineStr"/>
@@ -38660,7 +38660,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>581,64</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr"/>
@@ -39078,7 +39078,7 @@
       </c>
       <c r="G1017" t="inlineStr">
         <is>
-          <t>2032,6</t>
+          <t>612,6</t>
         </is>
       </c>
       <c r="H1017" t="inlineStr"/>
@@ -39116,7 +39116,7 @@
       </c>
       <c r="G1018" t="inlineStr">
         <is>
-          <t>636,00</t>
+          <t>1727,00</t>
         </is>
       </c>
       <c r="H1018" t="inlineStr"/>
@@ -39154,7 +39154,7 @@
       </c>
       <c r="G1019" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2359,00</t>
         </is>
       </c>
       <c r="H1019" t="inlineStr"/>
@@ -39192,7 +39192,7 @@
       </c>
       <c r="G1020" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1182,00</t>
         </is>
       </c>
       <c r="H1020" t="inlineStr"/>
@@ -39344,7 +39344,7 @@
       </c>
       <c r="G1024" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,6245</t>
         </is>
       </c>
       <c r="H1024" t="inlineStr"/>
@@ -64046,7 +64046,7 @@
       </c>
       <c r="G1667" t="inlineStr">
         <is>
-          <t>8,92</t>
+          <t>36,00</t>
         </is>
       </c>
       <c r="H1667" t="inlineStr">
@@ -64088,7 +64088,7 @@
       </c>
       <c r="G1668" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>23,00</t>
         </is>
       </c>
       <c r="H1668" t="inlineStr">
@@ -64130,52 +64130,10 @@
       </c>
       <c r="G1669" t="inlineStr">
         <is>
-          <t>23,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1669" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1670">
-      <c r="A1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F1670" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1670" t="inlineStr">
-        <is>
-          <t>16,00</t>
-        </is>
-      </c>
-      <c r="H1670" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX VALVE RATING FOR VALVE COMPARE
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1666"/>
+  <dimension ref="A1:H1633"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>23,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>19,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H225" t="inlineStr"/>
@@ -9590,7 +9590,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
@@ -10274,7 +10274,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H259" t="inlineStr"/>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H306" t="inlineStr"/>
@@ -12136,7 +12136,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H308" t="inlineStr"/>
@@ -12250,7 +12250,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H311" t="inlineStr"/>
@@ -12288,7 +12288,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H312" t="inlineStr"/>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>27,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H336" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>38,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>81,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H339" t="inlineStr"/>
@@ -13390,7 +13390,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>26,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H341" t="inlineStr"/>
@@ -16430,7 +16430,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H421" t="inlineStr"/>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H422" t="inlineStr"/>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H423" t="inlineStr"/>
@@ -17836,7 +17836,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H458" t="inlineStr"/>
@@ -17874,7 +17874,7 @@
       </c>
       <c r="G459" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H459" t="inlineStr"/>
@@ -17912,7 +17912,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H460" t="inlineStr"/>
@@ -17950,7 +17950,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>25,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H461" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>63,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>29,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H464" t="inlineStr"/>
@@ -18102,7 +18102,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H465" t="inlineStr"/>
@@ -26424,7 +26424,7 @@
       </c>
       <c r="G684" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H684" t="inlineStr"/>
@@ -26462,7 +26462,7 @@
       </c>
       <c r="G685" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H685" t="inlineStr"/>
@@ -26500,7 +26500,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H686" t="inlineStr"/>
@@ -36380,7 +36380,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H946" t="inlineStr"/>
@@ -41662,7 +41662,7 @@
       </c>
       <c r="G1085" t="inlineStr">
         <is>
-          <t>30,748</t>
+          <t>86,463</t>
         </is>
       </c>
       <c r="H1085" t="inlineStr"/>
@@ -41700,7 +41700,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>242,865</t>
+          <t>6,795</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr"/>
@@ -41738,7 +41738,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>1156,874</t>
+          <t>87,6</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr"/>
@@ -41776,7 +41776,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>3145,005</t>
+          <t>103,765</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr"/>
@@ -41814,7 +41814,7 @@
       </c>
       <c r="G1089" t="inlineStr">
         <is>
-          <t>763,336</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1089" t="inlineStr"/>
@@ -41852,7 +41852,7 @@
       </c>
       <c r="G1090" t="inlineStr">
         <is>
-          <t>1423,756</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1090" t="inlineStr"/>
@@ -41890,7 +41890,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>9224,864</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr"/>
@@ -41966,7 +41966,7 @@
       </c>
       <c r="G1093" t="inlineStr">
         <is>
-          <t>2143,774</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1093" t="inlineStr"/>
@@ -42004,7 +42004,7 @@
       </c>
       <c r="G1094" t="inlineStr">
         <is>
-          <t>1379,894</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1094" t="inlineStr"/>
@@ -42422,7 +42422,7 @@
       </c>
       <c r="G1105" t="inlineStr">
         <is>
-          <t>33,32</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1105" t="inlineStr"/>
@@ -42460,7 +42460,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>581,64</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr"/>
@@ -42878,7 +42878,7 @@
       </c>
       <c r="G1117" t="inlineStr">
         <is>
-          <t>36,6</t>
+          <t>35,1</t>
         </is>
       </c>
       <c r="H1117" t="inlineStr"/>
@@ -42916,7 +42916,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>82,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>475,00</t>
+          <t>29,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>225,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>539,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43068,7 +43068,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>1152,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -43106,7 +43106,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>2965,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr"/>
@@ -43182,7 +43182,7 @@
       </c>
       <c r="G1125" t="inlineStr">
         <is>
-          <t>406,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1125" t="inlineStr"/>
@@ -44018,7 +44018,7 @@
       </c>
       <c r="G1147" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1147" t="inlineStr"/>
@@ -44056,7 +44056,7 @@
       </c>
       <c r="G1148" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1148" t="inlineStr"/>
@@ -44094,7 +44094,7 @@
       </c>
       <c r="G1149" t="inlineStr">
         <is>
-          <t>19,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1149" t="inlineStr"/>
@@ -44132,7 +44132,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr"/>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr"/>
@@ -44208,7 +44208,7 @@
       </c>
       <c r="G1152" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1152" t="inlineStr"/>
@@ -44246,7 +44246,7 @@
       </c>
       <c r="G1153" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1153" t="inlineStr"/>
@@ -44322,7 +44322,7 @@
       </c>
       <c r="G1155" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1155" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>359,3</t>
+          <t>6,29</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>359,3</t>
+          <t>6,29</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>359,3</t>
+          <t>6,29</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>359,3</t>
+          <t>6,29</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -47476,7 +47476,7 @@
       </c>
       <c r="G1238" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>15,00</t>
         </is>
       </c>
       <c r="H1238" t="inlineStr"/>
@@ -47514,7 +47514,7 @@
       </c>
       <c r="G1239" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1239" t="inlineStr"/>
@@ -47552,7 +47552,7 @@
       </c>
       <c r="G1240" t="inlineStr">
         <is>
-          <t>23,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1240" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>5049,6</t>
+          <t>132,00</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>71,4</t>
+          <t>103,2</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>3168,375</t>
+          <t>39,6375</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -55418,7 +55418,7 @@
       </c>
       <c r="G1447" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1447" t="inlineStr"/>
@@ -57356,7 +57356,7 @@
       </c>
       <c r="G1498" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1498" t="inlineStr"/>
@@ -57394,7 +57394,7 @@
       </c>
       <c r="G1499" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1499" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>799,04</t>
+          <t>11,97</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW FEMALE END ASME B16.11 SW 3000# FORGED ASTM A105, 1/2"</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 2"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61316,7 +61316,7 @@
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -61348,7 +61348,7 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1"</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
@@ -61390,7 +61390,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-30</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -61400,7 +61400,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>20,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,7 +61432,7 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-30</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
@@ -61442,7 +61442,7 @@
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,17 +61474,17 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 2", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,17 +61516,17 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>28,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 1"</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61568,7 +61568,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>21,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -61600,7 +61600,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -61610,7 +61610,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>15,00</t>
+          <t>44,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,7 +61642,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X75MMLG</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -61652,7 +61652,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,7 +61684,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 3"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -61694,7 +61694,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>19,00</t>
+          <t>60,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,7 +61726,7 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
+          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 2"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
@@ -61736,7 +61736,7 @@
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,7 +61768,7 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 6"</t>
+          <t>SUMINISTRO DE LIFT CHECK VALVE SW, API 602, A105, CL 800, INST HORIZ/VERT, SW, B16.11, BOLTED COVER, SPW SS304/GRAPH, PISTON TYPE OBTURATOR, TRIM #8, 1/2"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
@@ -61778,7 +61778,7 @@
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,7 +61810,7 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1"</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 3"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
@@ -61820,7 +61820,7 @@
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -61852,7 +61852,7 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
@@ -61862,7 +61862,7 @@
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -61894,7 +61894,7 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11-1/2"</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
@@ -61936,17 +61936,17 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 10", S-30</t>
+          <t>SUMINISTRO DE INTEGRAL MONO FLANGE DBB NEEDLE MULTI-VALVE, EEMUA 182, A105, CL 150, RF/NPTF, B16.5 AND B1.20.1, BB, SPW SS304/GRAPH, PKG GRAPH; SS316 STEM, SEATS&amp;STEM TIP, S, SWIVEL NEEDLE, STEM OS&amp;Y/RSRO, T-HANDLE, 3/4"</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1617" t="inlineStr">
         <is>
-          <t>143,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1617" t="inlineStr">
@@ -61978,17 +61978,17 @@
       </c>
       <c r="E1618" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 14", S-30</t>
+          <t>SUMINISTRO DE SPECTACLE BLIND F8S ASME B16.48 WAFER JOINT TYPE 150 LB RAISED FACE FROM PLATE ASTM A516 GRADE 70, 1"</t>
         </is>
       </c>
       <c r="F1618" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1618" t="inlineStr">
         <is>
-          <t>23,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1618" t="inlineStr">
@@ -62020,17 +62020,17 @@
       </c>
       <c r="E1619" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 18", S-40</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS PIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 1/2"</t>
         </is>
       </c>
       <c r="F1619" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1619" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1619" t="inlineStr">
@@ -62062,17 +62062,17 @@
       </c>
       <c r="E1620" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
+          <t>SUMINISTRO DE GATE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SOLID WEDGE, STEM OS&amp;Y/RSNRO, HO, 3/4"</t>
         </is>
       </c>
       <c r="F1620" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1620" t="inlineStr">
         <is>
-          <t>25,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1620" t="inlineStr">
@@ -62104,17 +62104,17 @@
       </c>
       <c r="E1621" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
         </is>
       </c>
       <c r="F1621" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1621" t="inlineStr">
         <is>
-          <t>76,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1621" t="inlineStr">
@@ -62146,17 +62146,17 @@
       </c>
       <c r="E1622" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1622" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1622" t="inlineStr">
         <is>
-          <t>147,00</t>
+          <t>12,00</t>
         </is>
       </c>
       <c r="H1622" t="inlineStr">
@@ -62188,7 +62188,7 @@
       </c>
       <c r="E1623" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
         </is>
       </c>
       <c r="F1623" t="inlineStr">
@@ -62198,7 +62198,7 @@
       </c>
       <c r="G1623" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H1623" t="inlineStr">
@@ -62230,17 +62230,17 @@
       </c>
       <c r="E1624" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 1-1/2"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
         </is>
       </c>
       <c r="F1624" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1624" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1624" t="inlineStr">
@@ -62272,17 +62272,17 @@
       </c>
       <c r="E1625" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 10"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1625" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1625" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1625" t="inlineStr">
@@ -62314,7 +62314,7 @@
       </c>
       <c r="E1626" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 16"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 1"</t>
         </is>
       </c>
       <c r="F1626" t="inlineStr">
@@ -62356,7 +62356,7 @@
       </c>
       <c r="E1627" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 3/4"</t>
         </is>
       </c>
       <c r="F1627" t="inlineStr">
@@ -62398,7 +62398,7 @@
       </c>
       <c r="E1628" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 1"</t>
         </is>
       </c>
       <c r="F1628" t="inlineStr">
@@ -62408,7 +62408,7 @@
       </c>
       <c r="G1628" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1628" t="inlineStr">
@@ -62440,7 +62440,7 @@
       </c>
       <c r="E1629" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 3/4"</t>
         </is>
       </c>
       <c r="F1629" t="inlineStr">
@@ -62450,7 +62450,7 @@
       </c>
       <c r="G1629" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1629" t="inlineStr">
@@ -62482,7 +62482,7 @@
       </c>
       <c r="E1630" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1-1/2"</t>
+          <t>SUMINISTRO DE SW FLANGE, CLASS 150, RF, ASTM A105, ASME B16.5, 1/2"</t>
         </is>
       </c>
       <c r="F1630" t="inlineStr">
@@ -62524,7 +62524,7 @@
       </c>
       <c r="E1631" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X8"</t>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 40 X SCH 80, BWXPE, ASTM A-234 GR WCB, MSS SP-95 2"X1"</t>
         </is>
       </c>
       <c r="F1631" t="inlineStr">
@@ -62566,7 +62566,7 @@
       </c>
       <c r="E1632" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X8"</t>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 80 X SCH 80, PEXPE, ASTM A-234 GR WCB, MSS SP-95 1-1/2"X1"</t>
         </is>
       </c>
       <c r="F1632" t="inlineStr">
@@ -62576,7 +62576,7 @@
       </c>
       <c r="G1632" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1632" t="inlineStr">
@@ -62608,1406 +62608,20 @@
       </c>
       <c r="E1633" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 10"</t>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
         </is>
       </c>
       <c r="F1633" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1633" t="inlineStr">
         <is>
-          <t>38,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1633" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1634">
-      <c r="A1634" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1634" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1634" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1634" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1634" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 14"</t>
-        </is>
-      </c>
-      <c r="F1634" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1634" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1634" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1635">
-      <c r="A1635" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1635" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1635" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1635" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1635" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 16"</t>
-        </is>
-      </c>
-      <c r="F1635" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1635" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1635" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1636">
-      <c r="A1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1636" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 14"</t>
-        </is>
-      </c>
-      <c r="F1636" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1636" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1636" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1637">
-      <c r="A1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1637" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 10"</t>
-        </is>
-      </c>
-      <c r="F1637" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1637" t="inlineStr">
-        <is>
-          <t>11,00</t>
-        </is>
-      </c>
-      <c r="H1637" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1638">
-      <c r="A1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1638" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 2"</t>
-        </is>
-      </c>
-      <c r="F1638" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1638" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1638" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1639">
-      <c r="A1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1639" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 8"</t>
-        </is>
-      </c>
-      <c r="F1639" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1639" t="inlineStr">
-        <is>
-          <t>8,00</t>
-        </is>
-      </c>
-      <c r="H1639" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1640">
-      <c r="A1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1640" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GLOBE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PLUG DISC, STEM OS&amp;Y/RSRO, HO, 1/2"</t>
-        </is>
-      </c>
-      <c r="F1640" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1640" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1640" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1641">
-      <c r="A1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1641" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE GLOBE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PLUG DISC, STEM OS&amp;Y/RSRO, HO, 3/4"</t>
-        </is>
-      </c>
-      <c r="F1641" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1641" t="inlineStr">
-        <is>
-          <t>9,00</t>
-        </is>
-      </c>
-      <c r="H1641" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1642">
-      <c r="A1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1642" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1642" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1642" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1642" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1643">
-      <c r="A1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1643" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
-        </is>
-      </c>
-      <c r="F1643" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1643" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1643" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1644">
-      <c r="A1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1644" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
-        </is>
-      </c>
-      <c r="F1644" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1644" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1644" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1645">
-      <c r="A1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1645" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1-1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1645" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1645" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1645" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1646">
-      <c r="A1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1646" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1646" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1646" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1646" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1647">
-      <c r="A1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1647" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
-        </is>
-      </c>
-      <c r="F1647" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1647" t="inlineStr">
-        <is>
-          <t>6,00</t>
-        </is>
-      </c>
-      <c r="H1647" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1648">
-      <c r="A1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1648" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"X 8"</t>
-        </is>
-      </c>
-      <c r="F1648" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1648" t="inlineStr">
-        <is>
-          <t>9,00</t>
-        </is>
-      </c>
-      <c r="H1648" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1649">
-      <c r="A1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1649" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 10"X 6"</t>
-        </is>
-      </c>
-      <c r="F1649" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1649" t="inlineStr">
-        <is>
-          <t>7,00</t>
-        </is>
-      </c>
-      <c r="H1649" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1650">
-      <c r="A1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1650" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 10"</t>
-        </is>
-      </c>
-      <c r="F1650" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1650" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="H1650" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1651">
-      <c r="A1651" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1651" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1651" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1651" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1651" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 14"</t>
-        </is>
-      </c>
-      <c r="F1651" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1651" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1651" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1652">
-      <c r="A1652" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1652" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1652" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1652" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1652" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 1"</t>
-        </is>
-      </c>
-      <c r="F1652" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1652" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1652" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1653">
-      <c r="A1653" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1653" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1653" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1653" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1653" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 1-1/2"</t>
-        </is>
-      </c>
-      <c r="F1653" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1653" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1653" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1654">
-      <c r="A1654" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1654" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1654" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1654" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1654" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1654" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1654" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1654" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1655">
-      <c r="A1655" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1655" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1655" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1655" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1655" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 16" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1655" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1655" t="inlineStr">
-        <is>
-          <t>5,00</t>
-        </is>
-      </c>
-      <c r="H1655" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1656">
-      <c r="A1656" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1656" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1656" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1656" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1656" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 2" X 1/2"</t>
-        </is>
-      </c>
-      <c r="F1656" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1656" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1656" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1657">
-      <c r="A1657" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1657" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1657" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1657" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1657" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1657" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1657" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1657" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1658">
-      <c r="A1658" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1658" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1658" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1658" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1658" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 8" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1658" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1658" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1658" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1659">
-      <c r="A1659" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1659" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1659" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1659" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1659" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
-        </is>
-      </c>
-      <c r="F1659" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1659" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="H1659" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1660">
-      <c r="A1660" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1660" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1660" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1660" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1660" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 10"</t>
-        </is>
-      </c>
-      <c r="F1660" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1660" t="inlineStr">
-        <is>
-          <t>46,00</t>
-        </is>
-      </c>
-      <c r="H1660" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1661">
-      <c r="A1661" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1661" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1661" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1661" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1661" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 14"</t>
-        </is>
-      </c>
-      <c r="F1661" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1661" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1661" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1662">
-      <c r="A1662" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1662" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1662" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1662" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1662" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 40, RF, ASTM A-105, ASME B16.5 16"</t>
-        </is>
-      </c>
-      <c r="F1662" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1662" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1662" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1663">
-      <c r="A1663" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1663" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1663" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1663" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1663" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 10" X 2", S-30 X S-40</t>
-        </is>
-      </c>
-      <c r="F1663" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1663" t="inlineStr">
-        <is>
-          <t>11,00</t>
-        </is>
-      </c>
-      <c r="H1663" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1664">
-      <c r="A1664" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1664" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1664" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1664" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1664" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 10" X 3", S-30 X S-40</t>
-        </is>
-      </c>
-      <c r="F1664" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1664" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1664" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1665">
-      <c r="A1665" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1665" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1665" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1665" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1665" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 8" X 2", S-20 X S-40</t>
-        </is>
-      </c>
-      <c r="F1665" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1665" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1665" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1666">
-      <c r="A1666" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1666" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1666" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1666" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1666" t="inlineStr">
-        <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
-        </is>
-      </c>
-      <c r="F1666" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1666" t="inlineStr">
-        <is>
-          <t>16,00</t>
-        </is>
-      </c>
-      <c r="H1666" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX WEIGHT AND DESCRIPTION COMPARE
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1616"/>
+  <dimension ref="A1:H1635"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H225" t="inlineStr"/>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H306" t="inlineStr"/>
@@ -12136,7 +12136,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H308" t="inlineStr"/>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H336" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H422" t="inlineStr"/>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H423" t="inlineStr"/>
@@ -17836,7 +17836,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H458" t="inlineStr"/>
@@ -17874,7 +17874,7 @@
       </c>
       <c r="G459" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H459" t="inlineStr"/>
@@ -17950,7 +17950,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H461" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -26462,7 +26462,7 @@
       </c>
       <c r="G685" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H685" t="inlineStr"/>
@@ -36380,7 +36380,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H946" t="inlineStr"/>
@@ -41662,7 +41662,7 @@
       </c>
       <c r="G1085" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>86,463</t>
         </is>
       </c>
       <c r="H1085" t="inlineStr"/>
@@ -41700,7 +41700,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,795</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr"/>
@@ -41738,7 +41738,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>87,6</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr"/>
@@ -41776,7 +41776,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>103,765</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr"/>
@@ -42878,7 +42878,7 @@
       </c>
       <c r="G1117" t="inlineStr">
         <is>
-          <t>34,5</t>
+          <t>35,1</t>
         </is>
       </c>
       <c r="H1117" t="inlineStr"/>
@@ -42916,7 +42916,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>132,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>29,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>90,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>410,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43068,7 +43068,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>554,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -43106,7 +43106,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>532,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr"/>
@@ -43334,7 +43334,7 @@
       </c>
       <c r="G1129" t="inlineStr">
         <is>
-          <t>4512,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1129" t="inlineStr"/>
@@ -44018,7 +44018,7 @@
       </c>
       <c r="G1147" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1147" t="inlineStr"/>
@@ -44056,7 +44056,7 @@
       </c>
       <c r="G1148" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1148" t="inlineStr"/>
@@ -44094,7 +44094,7 @@
       </c>
       <c r="G1149" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1149" t="inlineStr"/>
@@ -44132,7 +44132,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr"/>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr"/>
@@ -44208,7 +44208,7 @@
       </c>
       <c r="G1152" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1152" t="inlineStr"/>
@@ -44246,7 +44246,7 @@
       </c>
       <c r="G1153" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1153" t="inlineStr"/>
@@ -44474,7 +44474,7 @@
       </c>
       <c r="G1159" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1159" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,39</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,39</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,39</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11,39</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>132,00</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>103,2</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>39,6375</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -55418,7 +55418,7 @@
       </c>
       <c r="G1447" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1447" t="inlineStr"/>
@@ -57356,7 +57356,7 @@
       </c>
       <c r="G1498" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1498" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>187,94</t>
+          <t>11,97</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW FEMALE END ASME B16.11 SW 3000# FORGED ASTM A105, 1/2"</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 6"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61358,7 +61358,7 @@
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -61390,7 +61390,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -61400,7 +61400,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,7 +61432,7 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
@@ -61442,7 +61442,7 @@
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,17 +61474,17 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 24"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,17 +61516,17 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 8"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 24"</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 1"</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61568,7 +61568,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -61600,7 +61600,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 8"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -61610,7 +61610,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>44,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,7 +61642,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GLOBE VALVE FL, API 623, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PARABOLIC DISC, STEM OS&amp;Y/RSRO, HO, 2"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X75MMLG</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -61652,7 +61652,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,7 +61684,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GLOBE VALVE FL, API 623, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SWIVEL PARABOLIC DISC, STEM OS&amp;Y/RSRO, HO, 6"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -61694,7 +61694,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>60,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,17 +61726,17 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
+          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 2"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>13,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,17 +61768,17 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SUMINISTRO DE LIFT CHECK VALVE SW, API 602, A105, CL 800, INST HORIZ/VERT, SW, B16.11, BOLTED COVER, SPW SS304/GRAPH, PISTON TYPE OBTURATOR, TRIM #8, 1/2"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,17 +61810,17 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 3"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -61852,17 +61852,17 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -61894,20 +61894,818 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11-1/2"</t>
+        </is>
+      </c>
+      <c r="F1616" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1616" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1616" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1617">
+      <c r="A1617" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F1616" t="inlineStr">
+      <c r="B1617" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G1616" t="inlineStr">
-        <is>
-          <t>13,00</t>
-        </is>
-      </c>
-      <c r="H1616" t="inlineStr">
+      <c r="C1617" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1617" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1617" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE INTEGRAL MONO FLANGE DBB NEEDLE MULTI-VALVE, EEMUA 182, A105, CL 150, RF/NPTF, B16.5 AND B1.20.1, BB, SPW SS304/GRAPH, PKG GRAPH; SS316 STEM, SEATS&amp;STEM TIP, S, SWIVEL NEEDLE, STEM OS&amp;Y/RSRO, T-HANDLE, 3/4"</t>
+        </is>
+      </c>
+      <c r="F1617" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1617" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="H1617" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1618" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1618" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SPECTACLE BLIND F8S ASME B16.48 WAFER JOINT TYPE 150 LB RAISED FACE FROM PLATE ASTM A516 GRADE 70, 1"</t>
+        </is>
+      </c>
+      <c r="F1618" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1618" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1618" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1619">
+      <c r="A1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1619" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1619" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS PIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 1/2"</t>
+        </is>
+      </c>
+      <c r="F1619" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1619" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1619" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1620" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1620" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE GATE VALVE SW, API 602, API 598, A105, CL 800, SW, B16.11, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, SOLID WEDGE, STEM OS&amp;Y/RSNRO, HO, 3/4"</t>
+        </is>
+      </c>
+      <c r="F1620" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1620" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1620" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1621" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1621" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
+        </is>
+      </c>
+      <c r="F1621" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1621" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="H1621" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1622">
+      <c r="A1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1622" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1622" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
+        </is>
+      </c>
+      <c r="F1622" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1622" t="inlineStr">
+        <is>
+          <t>12,00</t>
+        </is>
+      </c>
+      <c r="H1622" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1623">
+      <c r="A1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1623" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1623" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
+        </is>
+      </c>
+      <c r="F1623" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G1623" t="inlineStr">
+        <is>
+          <t>11,00</t>
+        </is>
+      </c>
+      <c r="H1623" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1624">
+      <c r="A1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1624" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1624" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
+        </is>
+      </c>
+      <c r="F1624" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G1624" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1624" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1625" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1625" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
+        </is>
+      </c>
+      <c r="F1625" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G1625" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1625" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1626" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1626" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 1"</t>
+        </is>
+      </c>
+      <c r="F1626" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1626" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1626" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1627" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1627" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 3/4"</t>
+        </is>
+      </c>
+      <c r="F1627" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1627" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="H1627" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1628" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1628" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 1"</t>
+        </is>
+      </c>
+      <c r="F1628" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1628" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1628" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1629" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1629" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 4" X 3/4"</t>
+        </is>
+      </c>
+      <c r="F1629" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1629" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1629" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1630" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1630" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE SW FLANGE, CLASS 150, RF, ASTM A105, ASME B16.5, 1/2"</t>
+        </is>
+      </c>
+      <c r="F1630" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1630" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1630" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1631" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1631" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 40 X SCH 80, BWXPE, ASTM A-234 GR WCB, MSS SP-95 2"X1"</t>
+        </is>
+      </c>
+      <c r="F1631" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1631" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1631" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1632" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1632" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE CONC. SWAGE, SCH 80 X SCH 80, PEXPE, ASTM A-234 GR WCB, MSS SP-95 1-1/2"X1"</t>
+        </is>
+      </c>
+      <c r="F1632" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1632" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1632" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1633" t="inlineStr">
+        <is>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
+        </is>
+      </c>
+      <c r="F1633" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1633" t="inlineStr">
+        <is>
+          <t>9,00</t>
+        </is>
+      </c>
+      <c r="H1633" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F1634" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1634" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1634" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F1635" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1635" t="inlineStr">
+        <is>
+          <t>15,00</t>
+        </is>
+      </c>
+      <c r="H1635" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
FIX DIAGNOSTIC FILE NO PIPING CLASS ELEMENTS
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1650"/>
+  <dimension ref="A1:H1635"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H163" t="inlineStr"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>26,00</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -10198,7 +10198,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H257" t="inlineStr"/>
@@ -10236,7 +10236,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H258" t="inlineStr"/>
@@ -10274,7 +10274,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H259" t="inlineStr"/>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H306" t="inlineStr"/>
@@ -12288,7 +12288,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H312" t="inlineStr"/>
@@ -12364,7 +12364,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H314" t="inlineStr"/>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H336" t="inlineStr"/>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H337" t="inlineStr"/>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H338" t="inlineStr"/>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H339" t="inlineStr"/>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H422" t="inlineStr"/>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H423" t="inlineStr"/>
@@ -17836,7 +17836,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H458" t="inlineStr"/>
@@ -17950,7 +17950,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H461" t="inlineStr"/>
@@ -17988,7 +17988,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H462" t="inlineStr"/>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H463" t="inlineStr"/>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H464" t="inlineStr"/>
@@ -18140,7 +18140,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H466" t="inlineStr"/>
@@ -18178,7 +18178,7 @@
       </c>
       <c r="G467" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H467" t="inlineStr"/>
@@ -18254,7 +18254,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H469" t="inlineStr"/>
@@ -18330,7 +18330,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H471" t="inlineStr"/>
@@ -18368,7 +18368,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H472" t="inlineStr"/>
@@ -18406,7 +18406,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H473" t="inlineStr"/>
@@ -21940,7 +21940,7 @@
       </c>
       <c r="G566" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H566" t="inlineStr"/>
@@ -26500,7 +26500,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H686" t="inlineStr"/>
@@ -36114,7 +36114,7 @@
       </c>
       <c r="G939" t="inlineStr">
         <is>
-          <t>40,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H939" t="inlineStr"/>
@@ -36342,7 +36342,7 @@
       </c>
       <c r="G945" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>28,00</t>
         </is>
       </c>
       <c r="H945" t="inlineStr"/>
@@ -36380,7 +36380,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H946" t="inlineStr"/>
@@ -36418,7 +36418,7 @@
       </c>
       <c r="G947" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H947" t="inlineStr"/>
@@ -41662,7 +41662,7 @@
       </c>
       <c r="G1085" t="inlineStr">
         <is>
-          <t>45,428</t>
+          <t>168,75</t>
         </is>
       </c>
       <c r="H1085" t="inlineStr"/>
@@ -41700,7 +41700,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>38,28</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr"/>
@@ -41738,7 +41738,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>382,418</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr"/>
@@ -41776,7 +41776,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>84,713</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr"/>
@@ -41814,7 +41814,7 @@
       </c>
       <c r="G1089" t="inlineStr">
         <is>
-          <t>853,644</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1089" t="inlineStr"/>
@@ -41852,7 +41852,7 @@
       </c>
       <c r="G1090" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>76,204</t>
         </is>
       </c>
       <c r="H1090" t="inlineStr"/>
@@ -41890,7 +41890,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2803,726</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr"/>
@@ -41928,7 +41928,7 @@
       </c>
       <c r="G1092" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>275,42</t>
         </is>
       </c>
       <c r="H1092" t="inlineStr"/>
@@ -42878,7 +42878,7 @@
       </c>
       <c r="G1117" t="inlineStr">
         <is>
-          <t>31,1</t>
+          <t>54,9</t>
         </is>
       </c>
       <c r="H1117" t="inlineStr"/>
@@ -42916,7 +42916,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>54,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -42954,7 +42954,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>147,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -42992,7 +42992,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>93,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -43030,7 +43030,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>77,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -43106,7 +43106,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>768,00</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr"/>
@@ -44018,7 +44018,7 @@
       </c>
       <c r="G1147" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1147" t="inlineStr"/>
@@ -44056,7 +44056,7 @@
       </c>
       <c r="G1148" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1148" t="inlineStr"/>
@@ -44094,7 +44094,7 @@
       </c>
       <c r="G1149" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1149" t="inlineStr"/>
@@ -44132,7 +44132,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr"/>
@@ -44170,7 +44170,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr"/>
@@ -44588,7 +44588,7 @@
       </c>
       <c r="G1162" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1162" t="inlineStr"/>
@@ -44626,7 +44626,7 @@
       </c>
       <c r="G1163" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1163" t="inlineStr"/>
@@ -44816,7 +44816,7 @@
       </c>
       <c r="G1168" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1168" t="inlineStr"/>
@@ -47058,7 +47058,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>28,04</t>
+          <t>46,79</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="G1229" t="inlineStr">
         <is>
-          <t>28,04</t>
+          <t>46,79</t>
         </is>
       </c>
       <c r="H1229" t="inlineStr"/>
@@ -47248,7 +47248,7 @@
       </c>
       <c r="G1232" t="inlineStr">
         <is>
-          <t>28,04</t>
+          <t>46,79</t>
         </is>
       </c>
       <c r="H1232" t="inlineStr"/>
@@ -47324,7 +47324,7 @@
       </c>
       <c r="G1234" t="inlineStr">
         <is>
-          <t>28,04</t>
+          <t>46,79</t>
         </is>
       </c>
       <c r="H1234" t="inlineStr"/>
@@ -47476,7 +47476,7 @@
       </c>
       <c r="G1238" t="inlineStr">
         <is>
-          <t>13,00</t>
+          <t>18,00</t>
         </is>
       </c>
       <c r="H1238" t="inlineStr"/>
@@ -47514,7 +47514,7 @@
       </c>
       <c r="G1239" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1239" t="inlineStr"/>
@@ -47552,7 +47552,7 @@
       </c>
       <c r="G1240" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1240" t="inlineStr"/>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="G1253" t="inlineStr">
         <is>
-          <t>639,6</t>
+          <t>832,8</t>
         </is>
       </c>
       <c r="H1253" t="inlineStr"/>
@@ -48084,7 +48084,7 @@
       </c>
       <c r="G1254" t="inlineStr">
         <is>
-          <t>53,1</t>
+          <t>135,3</t>
         </is>
       </c>
       <c r="H1254" t="inlineStr"/>
@@ -48198,7 +48198,7 @@
       </c>
       <c r="G1257" t="inlineStr">
         <is>
-          <t>217,6125</t>
+          <t>357,00</t>
         </is>
       </c>
       <c r="H1257" t="inlineStr"/>
@@ -57394,7 +57394,7 @@
       </c>
       <c r="G1499" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H1499" t="inlineStr"/>
@@ -61004,7 +61004,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>56,96</t>
+          <t>124,57</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr"/>
@@ -61222,7 +61222,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 3"</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -61232,7 +61232,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -61264,7 +61264,7 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
@@ -61274,7 +61274,7 @@
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -61306,7 +61306,7 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW FEMALE END ASME B16.11 SW 3000# FORGED ASTM A105, 1/2"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-20</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
@@ -61316,7 +61316,7 @@
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -61348,7 +61348,7 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 2", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1"</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
@@ -61358,7 +61358,7 @@
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -61390,7 +61390,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -61400,7 +61400,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>19,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -61432,17 +61432,17 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -61474,17 +61474,17 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
+          <t>SUMINISTRO DE PIPE, SCH 20, SMLS, BE, API 5L GR. B, PSL2, ASME B36.10, DIAM. 10"</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>28,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -61516,12 +61516,12 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 3"</t>
+          <t>SUMINISTRO DE PIPE, SCH 20, SMLS, BE, API 5L GR. B, PSL2, ASME B36.10, DIAM. 12"</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1607" t="inlineStr">
@@ -61558,7 +61558,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
+          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 300 LB RAISED FACE FORGED ASTM A105, 10"</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -61600,7 +61600,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 6"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1 1/8"X185MMLG</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -61610,7 +61610,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>32,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -61642,7 +61642,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X170MMLG</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -61652,7 +61652,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>288,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -61684,7 +61684,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1-1/2"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -61694,7 +61694,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -61726,7 +61726,7 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 1/2"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X75MMLG</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
@@ -61736,7 +61736,7 @@
       </c>
       <c r="G1612" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1612" t="inlineStr">
@@ -61768,7 +61768,7 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø7/8"X150MMLG</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
@@ -61778,7 +61778,7 @@
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -61810,12 +61810,12 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 300, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1614" t="inlineStr">
@@ -61852,17 +61852,17 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
+          <t>SUMINISTRO DE INTEGRAL MONO FLANGE DBB NEEDLE MULTI-VALVE, EEMUA 182, A105, CL 300, RF/NPTF, B16.5 AND B1.20.1, BB, SPW SS304/GRAPH, PKG GRAPH; SS316 STEM, SEATS&amp;STEM TIP, S, SWIVEL NEEDLE, STEM OS&amp;Y/RSRO, T-HANDLE, 3/4"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -61894,12 +61894,12 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X10"</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1616" t="inlineStr">
@@ -61936,12 +61936,12 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6", S-40</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 300 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 10"</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1617" t="inlineStr">
@@ -61978,7 +61978,7 @@
       </c>
       <c r="E1618" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BLIND FLANGE ASME B16.5 FLG 150 LB RAISED FACE FORGED ASTM A105, 1"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 300 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 12"</t>
         </is>
       </c>
       <c r="F1618" t="inlineStr">
@@ -61988,7 +61988,7 @@
       </c>
       <c r="G1618" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1618" t="inlineStr">
@@ -62020,7 +62020,7 @@
       </c>
       <c r="E1619" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 300, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 10"</t>
         </is>
       </c>
       <c r="F1619" t="inlineStr">
@@ -62030,7 +62030,7 @@
       </c>
       <c r="G1619" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1619" t="inlineStr">
@@ -62062,7 +62062,7 @@
       </c>
       <c r="E1620" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X75MMLG</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
         </is>
       </c>
       <c r="F1620" t="inlineStr">
@@ -62072,7 +62072,7 @@
       </c>
       <c r="G1620" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1620" t="inlineStr">
@@ -62104,7 +62104,7 @@
       </c>
       <c r="E1621" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X125MMLG</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1621" t="inlineStr">
@@ -62114,7 +62114,7 @@
       </c>
       <c r="G1621" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="H1621" t="inlineStr">
@@ -62146,17 +62146,17 @@
       </c>
       <c r="E1622" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X135MMLG</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
         </is>
       </c>
       <c r="F1622" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1622" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>32,00</t>
         </is>
       </c>
       <c r="H1622" t="inlineStr">
@@ -62188,17 +62188,17 @@
       </c>
       <c r="E1623" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
         </is>
       </c>
       <c r="F1623" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1623" t="inlineStr">
         <is>
-          <t>76,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1623" t="inlineStr">
@@ -62230,17 +62230,17 @@
       </c>
       <c r="E1624" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1624" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1624" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1624" t="inlineStr">
@@ -62272,7 +62272,7 @@
       </c>
       <c r="E1625" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CAP, SCH 40, SMLS, BW, ASTM A234 GR. WPB, ASME B16.9, 3"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 1"</t>
         </is>
       </c>
       <c r="F1625" t="inlineStr">
@@ -62282,7 +62282,7 @@
       </c>
       <c r="G1625" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1625" t="inlineStr">
@@ -62314,7 +62314,7 @@
       </c>
       <c r="E1626" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE LIFT CHECK VALVE SW, API 602, A105, CL 800, INST HORIZ/VERT, SW, B16.11, BOLTED COVER, SPW SS304/GRAPH, PISTON TYPE OBTURATOR, TRIM #8, 1/2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 10" X 3/4"</t>
         </is>
       </c>
       <c r="F1626" t="inlineStr">
@@ -62324,7 +62324,7 @@
       </c>
       <c r="G1626" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1626" t="inlineStr">
@@ -62356,7 +62356,7 @@
       </c>
       <c r="E1627" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 3"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 12" X 3/4"</t>
         </is>
       </c>
       <c r="F1627" t="inlineStr">
@@ -62366,7 +62366,7 @@
       </c>
       <c r="G1627" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1627" t="inlineStr">
@@ -62398,7 +62398,7 @@
       </c>
       <c r="E1628" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 4"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 2" X 1"</t>
         </is>
       </c>
       <c r="F1628" t="inlineStr">
@@ -62440,7 +62440,7 @@
       </c>
       <c r="E1629" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 300, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 2"</t>
+          <t>SUMINISTRO DE SW FLANGE, CLASS 300, RF, ASTM A105, ASME B16.5, 1"</t>
         </is>
       </c>
       <c r="F1629" t="inlineStr">
@@ -62450,7 +62450,7 @@
       </c>
       <c r="G1629" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1629" t="inlineStr">
@@ -62482,7 +62482,7 @@
       </c>
       <c r="E1630" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 3/4"</t>
+          <t>SUMINISTRO DE SW FLANGE, CLASS 300, RF, ASTM A105, ASME B16.5, 3/4"</t>
         </is>
       </c>
       <c r="F1630" t="inlineStr">
@@ -62492,7 +62492,7 @@
       </c>
       <c r="G1630" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1630" t="inlineStr">
@@ -62524,7 +62524,7 @@
       </c>
       <c r="E1631" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11-1/2"</t>
+          <t>SUMINISTRO DE TEE, SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
         </is>
       </c>
       <c r="F1631" t="inlineStr">
@@ -62534,7 +62534,7 @@
       </c>
       <c r="G1631" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1631" t="inlineStr">
@@ -62566,7 +62566,7 @@
       </c>
       <c r="E1632" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE INTEGRAL MONO FLANGE DBB NEEDLE MULTI-VALVE, EEMUA 182, A105, CL 150, RF/NPTF, B16.5 AND B1.20.1, BB, SPW SS304/GRAPH, PKG GRAPH; SS316 STEM, SEATS&amp;STEM TIP, S, SWIVEL NEEDLE, STEM OS&amp;Y/RSRO, T-HANDLE, 3/4"</t>
+          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 20, RF, ASTM A-105, ASME B16.5 10"</t>
         </is>
       </c>
       <c r="F1632" t="inlineStr">
@@ -62576,7 +62576,7 @@
       </c>
       <c r="G1632" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>21,00</t>
         </is>
       </c>
       <c r="H1632" t="inlineStr">
@@ -62608,7 +62608,7 @@
       </c>
       <c r="E1633" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS PIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 1/2"</t>
+          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 20, RF, ASTM A-105, ASME B16.5 12"</t>
         </is>
       </c>
       <c r="F1633" t="inlineStr">
@@ -62650,7 +62650,7 @@
       </c>
       <c r="E1634" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 2"</t>
+          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 20, RF, ASTM A-105, ASME B16.5 8"</t>
         </is>
       </c>
       <c r="F1634" t="inlineStr">
@@ -62660,7 +62660,7 @@
       </c>
       <c r="G1634" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1634" t="inlineStr">
@@ -62692,650 +62692,20 @@
       </c>
       <c r="E1635" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 3"</t>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
         </is>
       </c>
       <c r="F1635" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1635" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1635" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1636">
-      <c r="A1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1636" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1636" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
-        </is>
-      </c>
-      <c r="F1636" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1636" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1636" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1637">
-      <c r="A1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1637" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1637" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1-1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1637" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1637" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1637" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1638">
-      <c r="A1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1638" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1638" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1638" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1638" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1638" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1639">
-      <c r="A1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1639" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1639" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
-        </is>
-      </c>
-      <c r="F1639" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1639" t="inlineStr">
-        <is>
-          <t>7,00</t>
-        </is>
-      </c>
-      <c r="H1639" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1640">
-      <c r="A1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1640" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1640" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1/2", S-80</t>
-        </is>
-      </c>
-      <c r="F1640" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1640" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="H1640" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1641">
-      <c r="A1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1641" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1641" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 3/4", S-80</t>
-        </is>
-      </c>
-      <c r="F1641" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G1641" t="inlineStr">
-        <is>
-          <t>7,00</t>
-        </is>
-      </c>
-      <c r="H1641" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1642">
-      <c r="A1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1642" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1642" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE REDUCER TEE, CLASS 3000, SW, ASTM A105, ASME B.16.11, DIAM. 3/4"X1/2"</t>
-        </is>
-      </c>
-      <c r="F1642" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1642" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1642" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1643">
-      <c r="A1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1643" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1643" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 3" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1643" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1643" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="H1643" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1644">
-      <c r="A1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1644" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1644" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 6" X 1-1/2"</t>
-        </is>
-      </c>
-      <c r="F1644" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1644" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1644" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1645">
-      <c r="A1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1645" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1645" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 6" X 3/4"</t>
-        </is>
-      </c>
-      <c r="F1645" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1645" t="inlineStr">
-        <is>
-          <t>5,00</t>
-        </is>
-      </c>
-      <c r="H1645" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1646">
-      <c r="A1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1646" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1646" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE SW FLANGE, CLASS 150, RF, ASTM A105, ASME B16.5, 1/2"</t>
-        </is>
-      </c>
-      <c r="F1646" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1646" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="H1646" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1647">
-      <c r="A1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1647" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1647" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 80, RF, ASTM A-105, ASME B16.5 2"</t>
-        </is>
-      </c>
-      <c r="F1647" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1647" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="H1647" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1648">
-      <c r="A1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1648" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1648" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 80, RF, ASTM A-105, ASME B16.5 4"</t>
-        </is>
-      </c>
-      <c r="F1648" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1648" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1648" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1649">
-      <c r="A1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1649" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1649" t="inlineStr">
-        <is>
-          <t>SUMINISTRO DE FLANGE WN, 300#, SCH 80, RF, ASTM A-105, ASME B16.5 6"</t>
-        </is>
-      </c>
-      <c r="F1649" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="G1649" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="H1649" t="inlineStr">
-        <is>
-          <t>NUEVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="1650">
-      <c r="A1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E1650" t="inlineStr">
-        <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
-        </is>
-      </c>
-      <c r="F1650" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G1650" t="inlineStr">
-        <is>
-          <t>6,00</t>
-        </is>
-      </c>
-      <c r="H1650" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>

<commit_message>
SOLVE P&ID AND BOLTS DIMENSIONS
</commit_message>
<xml_diff>
--- a/output/co.xlsx
+++ b/output/co.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1682"/>
+  <dimension ref="A1:H1689"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>548,00</t>
+          <t>279,00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -6482,7 +6482,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H168" t="inlineStr"/>
@@ -6734,7 +6734,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>20,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H175" t="inlineStr"/>
@@ -7418,7 +7418,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H194" t="inlineStr"/>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H195" t="inlineStr"/>
@@ -7922,7 +7922,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H208" t="inlineStr"/>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H210" t="inlineStr"/>
@@ -8030,7 +8030,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H211" t="inlineStr"/>
@@ -8606,7 +8606,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H227" t="inlineStr"/>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H276" t="inlineStr"/>
@@ -11450,7 +11450,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H306" t="inlineStr"/>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H307" t="inlineStr"/>
@@ -11522,7 +11522,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H308" t="inlineStr"/>
@@ -11558,7 +11558,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H309" t="inlineStr"/>
@@ -11630,7 +11630,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>22,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H311" t="inlineStr"/>
@@ -14582,7 +14582,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H393" t="inlineStr"/>
@@ -15338,7 +15338,7 @@
       </c>
       <c r="G414" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H414" t="inlineStr"/>
@@ -15374,7 +15374,7 @@
       </c>
       <c r="G415" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H415" t="inlineStr"/>
@@ -15842,7 +15842,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H428" t="inlineStr"/>
@@ -15950,7 +15950,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H431" t="inlineStr"/>
@@ -15986,7 +15986,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H432" t="inlineStr"/>
@@ -16022,7 +16022,7 @@
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H433" t="inlineStr"/>
@@ -16058,7 +16058,7 @@
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H434" t="inlineStr"/>
@@ -16094,7 +16094,7 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>30,00</t>
+          <t>15,00</t>
         </is>
       </c>
       <c r="H435" t="inlineStr"/>
@@ -17966,7 +17966,7 @@
       </c>
       <c r="G487" t="inlineStr">
         <is>
-          <t>38,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H487" t="inlineStr"/>
@@ -33158,7 +33158,7 @@
       </c>
       <c r="G909" t="inlineStr">
         <is>
-          <t>400,00</t>
+          <t>200,00</t>
         </is>
       </c>
       <c r="H909" t="inlineStr"/>
@@ -33410,7 +33410,7 @@
       </c>
       <c r="G916" t="inlineStr">
         <is>
-          <t>72,00</t>
+          <t>36,00</t>
         </is>
       </c>
       <c r="H916" t="inlineStr"/>
@@ -33446,7 +33446,7 @@
       </c>
       <c r="G917" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H917" t="inlineStr"/>
@@ -33482,7 +33482,7 @@
       </c>
       <c r="G918" t="inlineStr">
         <is>
-          <t>144,00</t>
+          <t>120,00</t>
         </is>
       </c>
       <c r="H918" t="inlineStr"/>
@@ -34814,7 +34814,7 @@
       </c>
       <c r="G955" t="inlineStr">
         <is>
-          <t>558,308</t>
+          <t>279,154</t>
         </is>
       </c>
       <c r="H955" t="inlineStr"/>
@@ -34886,7 +34886,7 @@
       </c>
       <c r="G957" t="inlineStr">
         <is>
-          <t>54,24</t>
+          <t>27,12</t>
         </is>
       </c>
       <c r="H957" t="inlineStr"/>
@@ -34922,7 +34922,7 @@
       </c>
       <c r="G958" t="inlineStr">
         <is>
-          <t>1411,22</t>
+          <t>705,61</t>
         </is>
       </c>
       <c r="H958" t="inlineStr"/>
@@ -34958,7 +34958,7 @@
       </c>
       <c r="G959" t="inlineStr">
         <is>
-          <t>3397,92</t>
+          <t>1698,96</t>
         </is>
       </c>
       <c r="H959" t="inlineStr"/>
@@ -34994,7 +34994,7 @@
       </c>
       <c r="G960" t="inlineStr">
         <is>
-          <t>2406,78</t>
+          <t>1203,39</t>
         </is>
       </c>
       <c r="H960" t="inlineStr"/>
@@ -35030,7 +35030,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>214,3</t>
+          <t>107,15</t>
         </is>
       </c>
       <c r="H961" t="inlineStr"/>
@@ -35966,7 +35966,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>2152,00</t>
+          <t>1076,00</t>
         </is>
       </c>
       <c r="H987" t="inlineStr"/>
@@ -38414,7 +38414,7 @@
       </c>
       <c r="G1055" t="inlineStr">
         <is>
-          <t>73,736</t>
+          <t>33,928</t>
         </is>
       </c>
       <c r="H1055" t="inlineStr"/>
@@ -38450,7 +38450,7 @@
       </c>
       <c r="G1056" t="inlineStr">
         <is>
-          <t>58,084</t>
+          <t>33,038</t>
         </is>
       </c>
       <c r="H1056" t="inlineStr"/>
@@ -38486,7 +38486,7 @@
       </c>
       <c r="G1057" t="inlineStr">
         <is>
-          <t>100,372</t>
+          <t>54,886</t>
         </is>
       </c>
       <c r="H1057" t="inlineStr"/>
@@ -38522,7 +38522,7 @@
       </c>
       <c r="G1058" t="inlineStr">
         <is>
-          <t>4635,34</t>
+          <t>477,725</t>
         </is>
       </c>
       <c r="H1058" t="inlineStr"/>
@@ -38558,7 +38558,7 @@
       </c>
       <c r="G1059" t="inlineStr">
         <is>
-          <t>45655,676</t>
+          <t>22695,942</t>
         </is>
       </c>
       <c r="H1059" t="inlineStr"/>
@@ -38594,7 +38594,7 @@
       </c>
       <c r="G1060" t="inlineStr">
         <is>
-          <t>20459,004</t>
+          <t>10502,574</t>
         </is>
       </c>
       <c r="H1060" t="inlineStr"/>
@@ -38630,7 +38630,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>2041,74</t>
+          <t>1072,99</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr"/>
@@ -38666,7 +38666,7 @@
       </c>
       <c r="G1062" t="inlineStr">
         <is>
-          <t>2471,624</t>
+          <t>1473,166</t>
         </is>
       </c>
       <c r="H1062" t="inlineStr"/>
@@ -38702,7 +38702,7 @@
       </c>
       <c r="G1063" t="inlineStr">
         <is>
-          <t>70914,584</t>
+          <t>35973,25</t>
         </is>
       </c>
       <c r="H1063" t="inlineStr"/>
@@ -38738,7 +38738,7 @@
       </c>
       <c r="G1064" t="inlineStr">
         <is>
-          <t>49880,024</t>
+          <t>24901,792</t>
         </is>
       </c>
       <c r="H1064" t="inlineStr"/>
@@ -38846,7 +38846,7 @@
       </c>
       <c r="G1067" t="inlineStr">
         <is>
-          <t>178180,912</t>
+          <t>89340,26</t>
         </is>
       </c>
       <c r="H1067" t="inlineStr"/>
@@ -39566,7 +39566,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>12,00</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr"/>
@@ -39602,7 +39602,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>158,00</t>
+          <t>79,00</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr"/>
@@ -39638,7 +39638,7 @@
       </c>
       <c r="G1089" t="inlineStr">
         <is>
-          <t>300,00</t>
+          <t>150,00</t>
         </is>
       </c>
       <c r="H1089" t="inlineStr"/>
@@ -39674,7 +39674,7 @@
       </c>
       <c r="G1090" t="inlineStr">
         <is>
-          <t>90,00</t>
+          <t>45,00</t>
         </is>
       </c>
       <c r="H1090" t="inlineStr"/>
@@ -39710,7 +39710,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>176,00</t>
+          <t>360,00</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr"/>
@@ -39746,7 +39746,7 @@
       </c>
       <c r="G1092" t="inlineStr">
         <is>
-          <t>842,00</t>
+          <t>525,00</t>
         </is>
       </c>
       <c r="H1092" t="inlineStr"/>
@@ -39782,7 +39782,7 @@
       </c>
       <c r="G1093" t="inlineStr">
         <is>
-          <t>1064,00</t>
+          <t>532,00</t>
         </is>
       </c>
       <c r="H1093" t="inlineStr"/>
@@ -39818,7 +39818,7 @@
       </c>
       <c r="G1094" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>894,00</t>
         </is>
       </c>
       <c r="H1094" t="inlineStr"/>
@@ -39854,7 +39854,7 @@
       </c>
       <c r="G1095" t="inlineStr">
         <is>
-          <t>10986,00</t>
+          <t>5493,00</t>
         </is>
       </c>
       <c r="H1095" t="inlineStr"/>
@@ -39890,7 +39890,7 @@
       </c>
       <c r="G1096" t="inlineStr">
         <is>
-          <t>6104,00</t>
+          <t>3052,00</t>
         </is>
       </c>
       <c r="H1096" t="inlineStr"/>
@@ -39998,7 +39998,7 @@
       </c>
       <c r="G1099" t="inlineStr">
         <is>
-          <t>6320,00</t>
+          <t>3160,00</t>
         </is>
       </c>
       <c r="H1099" t="inlineStr"/>
@@ -40682,7 +40682,7 @@
       </c>
       <c r="G1118" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1118" t="inlineStr"/>
@@ -40718,7 +40718,7 @@
       </c>
       <c r="G1119" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1119" t="inlineStr"/>
@@ -40754,7 +40754,7 @@
       </c>
       <c r="G1120" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1120" t="inlineStr"/>
@@ -40790,7 +40790,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr"/>
@@ -40826,7 +40826,7 @@
       </c>
       <c r="G1122" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1122" t="inlineStr"/>
@@ -40862,7 +40862,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr"/>
@@ -40898,7 +40898,7 @@
       </c>
       <c r="G1124" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1124" t="inlineStr"/>
@@ -40934,7 +40934,7 @@
       </c>
       <c r="G1125" t="inlineStr">
         <is>
-          <t>30,00</t>
+          <t>15,00</t>
         </is>
       </c>
       <c r="H1125" t="inlineStr"/>
@@ -40970,7 +40970,7 @@
       </c>
       <c r="G1126" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1126" t="inlineStr"/>
@@ -41078,7 +41078,7 @@
       </c>
       <c r="G1129" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1129" t="inlineStr"/>
@@ -43526,7 +43526,7 @@
       </c>
       <c r="G1197" t="inlineStr">
         <is>
-          <t>5063,56</t>
+          <t>2484,59</t>
         </is>
       </c>
       <c r="H1197" t="inlineStr"/>
@@ -43598,7 +43598,7 @@
       </c>
       <c r="G1199" t="inlineStr">
         <is>
-          <t>5063,56</t>
+          <t>2484,59</t>
         </is>
       </c>
       <c r="H1199" t="inlineStr"/>
@@ -43706,7 +43706,7 @@
       </c>
       <c r="G1202" t="inlineStr">
         <is>
-          <t>5063,56</t>
+          <t>2484,59</t>
         </is>
       </c>
       <c r="H1202" t="inlineStr"/>
@@ -43778,7 +43778,7 @@
       </c>
       <c r="G1204" t="inlineStr">
         <is>
-          <t>5063,56</t>
+          <t>2484,59</t>
         </is>
       </c>
       <c r="H1204" t="inlineStr"/>
@@ -43922,7 +43922,7 @@
       </c>
       <c r="G1208" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1208" t="inlineStr"/>
@@ -43958,7 +43958,7 @@
       </c>
       <c r="G1209" t="inlineStr">
         <is>
-          <t>78,00</t>
+          <t>43,00</t>
         </is>
       </c>
       <c r="H1209" t="inlineStr"/>
@@ -43994,7 +43994,7 @@
       </c>
       <c r="G1210" t="inlineStr">
         <is>
-          <t>40,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1210" t="inlineStr"/>
@@ -44030,7 +44030,7 @@
       </c>
       <c r="G1211" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1211" t="inlineStr"/>
@@ -44462,7 +44462,7 @@
       </c>
       <c r="G1223" t="inlineStr">
         <is>
-          <t>10264,8</t>
+          <t>5216,88</t>
         </is>
       </c>
       <c r="H1223" t="inlineStr"/>
@@ -44498,7 +44498,7 @@
       </c>
       <c r="G1224" t="inlineStr">
         <is>
-          <t>333,6</t>
+          <t>169,2</t>
         </is>
       </c>
       <c r="H1224" t="inlineStr"/>
@@ -44606,7 +44606,7 @@
       </c>
       <c r="G1227" t="inlineStr">
         <is>
-          <t>54306,00</t>
+          <t>26633,25</t>
         </is>
       </c>
       <c r="H1227" t="inlineStr"/>
@@ -51518,7 +51518,7 @@
       </c>
       <c r="G1419" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1419" t="inlineStr"/>
@@ -56738,7 +56738,7 @@
       </c>
       <c r="G1564" t="inlineStr">
         <is>
-          <t>12039,65</t>
+          <t>6037,97</t>
         </is>
       </c>
       <c r="H1564" t="inlineStr"/>
@@ -56956,7 +56956,7 @@
       </c>
       <c r="G1570" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1570" t="inlineStr">
@@ -56988,7 +56988,7 @@
       </c>
       <c r="E1571" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 4"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
         </is>
       </c>
       <c r="F1571" t="inlineStr">
@@ -56998,7 +56998,7 @@
       </c>
       <c r="G1571" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1571" t="inlineStr">
@@ -57030,7 +57030,7 @@
       </c>
       <c r="E1572" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 6"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
         </is>
       </c>
       <c r="F1572" t="inlineStr">
@@ -57040,7 +57040,7 @@
       </c>
       <c r="G1572" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H1572" t="inlineStr">
@@ -57072,7 +57072,7 @@
       </c>
       <c r="E1573" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
+          <t>SUMINISTRO DE ELBOW 45° LR, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"</t>
         </is>
       </c>
       <c r="F1573" t="inlineStr">
@@ -57082,7 +57082,7 @@
       </c>
       <c r="G1573" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1573" t="inlineStr">
@@ -57114,7 +57114,7 @@
       </c>
       <c r="E1574" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ELBOW 45° LR, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-30</t>
         </is>
       </c>
       <c r="F1574" t="inlineStr">
@@ -57124,7 +57124,7 @@
       </c>
       <c r="G1574" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1574" t="inlineStr">
@@ -57156,7 +57156,7 @@
       </c>
       <c r="E1575" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 10", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 12", S-20</t>
         </is>
       </c>
       <c r="F1575" t="inlineStr">
@@ -57198,7 +57198,7 @@
       </c>
       <c r="E1576" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 12", S-20</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-30</t>
         </is>
       </c>
       <c r="F1576" t="inlineStr">
@@ -57208,7 +57208,7 @@
       </c>
       <c r="G1576" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1576" t="inlineStr">
@@ -57240,7 +57240,7 @@
       </c>
       <c r="E1577" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-STD</t>
         </is>
       </c>
       <c r="F1577" t="inlineStr">
@@ -57250,7 +57250,7 @@
       </c>
       <c r="G1577" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>31,00</t>
         </is>
       </c>
       <c r="H1577" t="inlineStr">
@@ -57282,7 +57282,7 @@
       </c>
       <c r="E1578" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 14", S-STD</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 16", S-STD</t>
         </is>
       </c>
       <c r="F1578" t="inlineStr">
@@ -57292,7 +57292,7 @@
       </c>
       <c r="G1578" t="inlineStr">
         <is>
-          <t>62,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1578" t="inlineStr">
@@ -57324,7 +57324,7 @@
       </c>
       <c r="E1579" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 16", S-STD</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 24", S-30</t>
         </is>
       </c>
       <c r="F1579" t="inlineStr">
@@ -57334,7 +57334,7 @@
       </c>
       <c r="G1579" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="H1579" t="inlineStr">
@@ -57366,7 +57366,7 @@
       </c>
       <c r="E1580" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 24", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
         </is>
       </c>
       <c r="F1580" t="inlineStr">
@@ -57376,7 +57376,7 @@
       </c>
       <c r="G1580" t="inlineStr">
         <is>
-          <t>22,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1580" t="inlineStr">
@@ -57408,7 +57408,7 @@
       </c>
       <c r="E1581" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 3", S-40</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
         </is>
       </c>
       <c r="F1581" t="inlineStr">
@@ -57418,7 +57418,7 @@
       </c>
       <c r="G1581" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1581" t="inlineStr">
@@ -57450,7 +57450,7 @@
       </c>
       <c r="E1582" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-30</t>
+          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
         </is>
       </c>
       <c r="F1582" t="inlineStr">
@@ -57460,7 +57460,7 @@
       </c>
       <c r="G1582" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>45,00</t>
         </is>
       </c>
       <c r="H1582" t="inlineStr">
@@ -57492,7 +57492,7 @@
       </c>
       <c r="E1583" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 4", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
         </is>
       </c>
       <c r="F1583" t="inlineStr">
@@ -57502,7 +57502,7 @@
       </c>
       <c r="G1583" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1583" t="inlineStr">
@@ -57534,7 +57534,7 @@
       </c>
       <c r="E1584" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE 90 DEGREE ELBOW LR ASME B16.9 BW WROUGHT S ASTM A234 GR. WPB, 6", S-40</t>
+          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
         </is>
       </c>
       <c r="F1584" t="inlineStr">
@@ -57544,7 +57544,7 @@
       </c>
       <c r="G1584" t="inlineStr">
         <is>
-          <t>70,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1584" t="inlineStr">
@@ -57576,7 +57576,7 @@
       </c>
       <c r="E1585" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 2"</t>
+          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
         </is>
       </c>
       <c r="F1585" t="inlineStr">
@@ -57586,7 +57586,7 @@
       </c>
       <c r="G1585" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1585" t="inlineStr">
@@ -57618,17 +57618,17 @@
       </c>
       <c r="E1586" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE FL, FB, LP, FLOATING BALL, API 608, A216 GR.WCB, CL 150, RF, B16.5, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, SPW SS304/GRAPH, API 607, LO, 4"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 10", S-30</t>
         </is>
       </c>
       <c r="F1586" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1586" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1586" t="inlineStr">
@@ -57660,17 +57660,17 @@
       </c>
       <c r="E1587" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE BALL VALVE W/INTEGRAL WELDED 2 NIPPLES, FB, FLOATING BALL, API 608, API 598, A105, CL 800, SW W/2 PE NIPPLES, MNF STD, SS316 BALL, SS316 STEM, 2 OR 3 PCS SPLIT BODY SIDE ENTRY, API 607, LO, 3/4"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 14", S-30</t>
         </is>
       </c>
       <c r="F1587" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1587" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>12,00</t>
         </is>
       </c>
       <c r="H1587" t="inlineStr">
@@ -57702,7 +57702,7 @@
       </c>
       <c r="E1588" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 10", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 18", S-40</t>
         </is>
       </c>
       <c r="F1588" t="inlineStr">
@@ -57712,7 +57712,7 @@
       </c>
       <c r="G1588" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1588" t="inlineStr">
@@ -57744,7 +57744,7 @@
       </c>
       <c r="E1589" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 14", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
         </is>
       </c>
       <c r="F1589" t="inlineStr">
@@ -57754,7 +57754,7 @@
       </c>
       <c r="G1589" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1589" t="inlineStr">
@@ -57786,7 +57786,7 @@
       </c>
       <c r="E1590" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 18", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 24", S-30</t>
         </is>
       </c>
       <c r="F1590" t="inlineStr">
@@ -57796,7 +57796,7 @@
       </c>
       <c r="G1590" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>386,00</t>
         </is>
       </c>
       <c r="H1590" t="inlineStr">
@@ -57828,7 +57828,7 @@
       </c>
       <c r="E1591" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 2", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
         </is>
       </c>
       <c r="F1591" t="inlineStr">
@@ -57838,7 +57838,7 @@
       </c>
       <c r="G1591" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1591" t="inlineStr">
@@ -57870,7 +57870,7 @@
       </c>
       <c r="E1592" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 24", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
         </is>
       </c>
       <c r="F1592" t="inlineStr">
@@ -57880,7 +57880,7 @@
       </c>
       <c r="G1592" t="inlineStr">
         <is>
-          <t>772,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1592" t="inlineStr">
@@ -57912,7 +57912,7 @@
       </c>
       <c r="E1593" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 3", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6", S-40</t>
         </is>
       </c>
       <c r="F1593" t="inlineStr">
@@ -57922,7 +57922,7 @@
       </c>
       <c r="G1593" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>19,00</t>
         </is>
       </c>
       <c r="H1593" t="inlineStr">
@@ -57954,7 +57954,7 @@
       </c>
       <c r="E1594" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 4", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 12", S-20</t>
         </is>
       </c>
       <c r="F1594" t="inlineStr">
@@ -57964,7 +57964,7 @@
       </c>
       <c r="G1594" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>18,00</t>
         </is>
       </c>
       <c r="H1594" t="inlineStr">
@@ -57996,7 +57996,7 @@
       </c>
       <c r="E1595" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A106 GR.  B, 6", S-40</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 14", S-STD</t>
         </is>
       </c>
       <c r="F1595" t="inlineStr">
@@ -58006,7 +58006,7 @@
       </c>
       <c r="G1595" t="inlineStr">
         <is>
-          <t>328,00</t>
+          <t>351,00</t>
         </is>
       </c>
       <c r="H1595" t="inlineStr">
@@ -58038,7 +58038,7 @@
       </c>
       <c r="E1596" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 12", S-20</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 16", S-STD</t>
         </is>
       </c>
       <c r="F1596" t="inlineStr">
@@ -58048,7 +58048,7 @@
       </c>
       <c r="G1596" t="inlineStr">
         <is>
-          <t>36,00</t>
+          <t>226,00</t>
         </is>
       </c>
       <c r="H1596" t="inlineStr">
@@ -58080,7 +58080,7 @@
       </c>
       <c r="E1597" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 14", S-STD</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2-1/2", S-30</t>
         </is>
       </c>
       <c r="F1597" t="inlineStr">
@@ -58090,7 +58090,7 @@
       </c>
       <c r="G1597" t="inlineStr">
         <is>
-          <t>690,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1597" t="inlineStr">
@@ -58122,7 +58122,7 @@
       </c>
       <c r="E1598" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 16", S-STD</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 4", S-30</t>
         </is>
       </c>
       <c r="F1598" t="inlineStr">
@@ -58132,7 +58132,7 @@
       </c>
       <c r="G1598" t="inlineStr">
         <is>
-          <t>452,00</t>
+          <t>20,00</t>
         </is>
       </c>
       <c r="H1598" t="inlineStr">
@@ -58164,7 +58164,7 @@
       </c>
       <c r="E1599" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 2-1/2", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 6", S-40</t>
         </is>
       </c>
       <c r="F1599" t="inlineStr">
@@ -58174,7 +58174,7 @@
       </c>
       <c r="G1599" t="inlineStr">
         <is>
-          <t>20,00</t>
+          <t>748,00</t>
         </is>
       </c>
       <c r="H1599" t="inlineStr">
@@ -58206,7 +58206,7 @@
       </c>
       <c r="E1600" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 4", S-30</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 8", S-20</t>
         </is>
       </c>
       <c r="F1600" t="inlineStr">
@@ -58216,7 +58216,7 @@
       </c>
       <c r="G1600" t="inlineStr">
         <is>
-          <t>322,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1600" t="inlineStr">
@@ -58248,17 +58248,17 @@
       </c>
       <c r="E1601" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 6", S-40</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1 3/8"X190MMLG</t>
         </is>
       </c>
       <c r="F1601" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1601" t="inlineStr">
         <is>
-          <t>1224,00</t>
+          <t>200,00</t>
         </is>
       </c>
       <c r="H1601" t="inlineStr">
@@ -58290,17 +58290,17 @@
       </c>
       <c r="E1602" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 BE SEAMLESS ASTM A53 GR.  B, 8", S-20</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X145MMLG</t>
         </is>
       </c>
       <c r="F1602" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1602" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>252,00</t>
         </is>
       </c>
       <c r="H1602" t="inlineStr">
@@ -58332,7 +58332,7 @@
       </c>
       <c r="E1603" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1 3/8"X190MMLG</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X150MMLG</t>
         </is>
       </c>
       <c r="F1603" t="inlineStr">
@@ -58342,7 +58342,7 @@
       </c>
       <c r="G1603" t="inlineStr">
         <is>
-          <t>240,00</t>
+          <t>208,00</t>
         </is>
       </c>
       <c r="H1603" t="inlineStr">
@@ -58374,7 +58374,7 @@
       </c>
       <c r="E1604" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X145MMLG</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
         </is>
       </c>
       <c r="F1604" t="inlineStr">
@@ -58384,7 +58384,7 @@
       </c>
       <c r="G1604" t="inlineStr">
         <is>
-          <t>864,00</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="H1604" t="inlineStr">
@@ -58416,7 +58416,7 @@
       </c>
       <c r="E1605" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1"X150MMLG</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X120MMLG</t>
         </is>
       </c>
       <c r="F1605" t="inlineStr">
@@ -58426,7 +58426,7 @@
       </c>
       <c r="G1605" t="inlineStr">
         <is>
-          <t>448,00</t>
+          <t>160,00</t>
         </is>
       </c>
       <c r="H1605" t="inlineStr">
@@ -58458,7 +58458,7 @@
       </c>
       <c r="E1606" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø1/2"X70MMLG</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
         </is>
       </c>
       <c r="F1606" t="inlineStr">
@@ -58468,7 +58468,7 @@
       </c>
       <c r="G1606" t="inlineStr">
         <is>
-          <t>32,00</t>
+          <t>128,00</t>
         </is>
       </c>
       <c r="H1606" t="inlineStr">
@@ -58500,7 +58500,7 @@
       </c>
       <c r="E1607" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø3/4"X120MMLG</t>
+          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø7/8"X135MMLG</t>
         </is>
       </c>
       <c r="F1607" t="inlineStr">
@@ -58510,7 +58510,7 @@
       </c>
       <c r="G1607" t="inlineStr">
         <is>
-          <t>288,00</t>
+          <t>18,00</t>
         </is>
       </c>
       <c r="H1607" t="inlineStr">
@@ -58542,7 +58542,7 @@
       </c>
       <c r="E1608" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø5/8"X100MMLG</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
         </is>
       </c>
       <c r="F1608" t="inlineStr">
@@ -58552,7 +58552,7 @@
       </c>
       <c r="G1608" t="inlineStr">
         <is>
-          <t>240,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1608" t="inlineStr">
@@ -58584,7 +58584,7 @@
       </c>
       <c r="E1609" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE STUD BOLTS, A-193 GR B7 W/(2) HVY NUTS HEX, ASTM A-194 GR 2H, ASME B18.2.1, B18.2.2 Ø7/8"X135MMLG</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 14"</t>
         </is>
       </c>
       <c r="F1609" t="inlineStr">
@@ -58594,7 +58594,7 @@
       </c>
       <c r="G1609" t="inlineStr">
         <is>
-          <t>24,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1609" t="inlineStr">
@@ -58626,7 +58626,7 @@
       </c>
       <c r="E1610" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 10"</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 24"</t>
         </is>
       </c>
       <c r="F1610" t="inlineStr">
@@ -58636,7 +58636,7 @@
       </c>
       <c r="G1610" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1610" t="inlineStr">
@@ -58668,7 +58668,7 @@
       </c>
       <c r="E1611" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 14"</t>
+          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 8"</t>
         </is>
       </c>
       <c r="F1611" t="inlineStr">
@@ -58678,7 +58678,7 @@
       </c>
       <c r="G1611" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1611" t="inlineStr">
@@ -58710,7 +58710,7 @@
       </c>
       <c r="E1612" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 24"</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1"</t>
         </is>
       </c>
       <c r="F1612" t="inlineStr">
@@ -58752,7 +58752,7 @@
       </c>
       <c r="E1613" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SWING CHECK VALVE FL, API 594, API 598, A216 GR.WCB, CL 150, INST HORIZ/VERT, RF, B16.5, BOLTED COVER, SPW SS304/GRAPH, RENEWABLE SEATS, TRIM #8, 8"</t>
+          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 3/4"</t>
         </is>
       </c>
       <c r="F1613" t="inlineStr">
@@ -58762,7 +58762,7 @@
       </c>
       <c r="G1613" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1613" t="inlineStr">
@@ -58794,7 +58794,7 @@
       </c>
       <c r="E1614" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 1"</t>
+          <t>SUMINISTRO DE CONC. REDUCER, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X4"</t>
         </is>
       </c>
       <c r="F1614" t="inlineStr">
@@ -58804,7 +58804,7 @@
       </c>
       <c r="G1614" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1614" t="inlineStr">
@@ -58836,7 +58836,7 @@
       </c>
       <c r="E1615" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE COUPLING, CLASS 3000, SW, ASTM A-105, ASME B16.11 3/4"</t>
+          <t>SUMINISTRO DE CONC. REDUCER, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X6"</t>
         </is>
       </c>
       <c r="F1615" t="inlineStr">
@@ -58846,7 +58846,7 @@
       </c>
       <c r="G1615" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1615" t="inlineStr">
@@ -58878,7 +58878,7 @@
       </c>
       <c r="E1616" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X4"</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 20 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X8"</t>
         </is>
       </c>
       <c r="F1616" t="inlineStr">
@@ -58888,7 +58888,7 @@
       </c>
       <c r="G1616" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1616" t="inlineStr">
@@ -58920,7 +58920,7 @@
       </c>
       <c r="E1617" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE CONC. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X4"</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X2-1/2"</t>
         </is>
       </c>
       <c r="F1617" t="inlineStr">
@@ -58962,7 +58962,7 @@
       </c>
       <c r="E1618" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 20 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 12"X8"</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X4"</t>
         </is>
       </c>
       <c r="F1618" t="inlineStr">
@@ -58972,7 +58972,7 @@
       </c>
       <c r="G1618" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1618" t="inlineStr">
@@ -59004,7 +59004,7 @@
       </c>
       <c r="E1619" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE EXCEN. REDUCER, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X2-1/2"</t>
+          <t>SUMINISTRO DE EXCEN. REDUCER, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"X14"</t>
         </is>
       </c>
       <c r="F1619" t="inlineStr">
@@ -59014,7 +59014,7 @@
       </c>
       <c r="G1619" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1619" t="inlineStr">
@@ -59046,7 +59046,7 @@
       </c>
       <c r="E1620" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE EXCEN. REDUCER, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"X14"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 12"</t>
         </is>
       </c>
       <c r="F1620" t="inlineStr">
@@ -59056,7 +59056,7 @@
       </c>
       <c r="G1620" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1620" t="inlineStr">
@@ -59088,7 +59088,7 @@
       </c>
       <c r="E1621" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 12"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 14"</t>
         </is>
       </c>
       <c r="F1621" t="inlineStr">
@@ -59098,7 +59098,7 @@
       </c>
       <c r="G1621" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1621" t="inlineStr">
@@ -59130,7 +59130,7 @@
       </c>
       <c r="E1622" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 14"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 16"</t>
         </is>
       </c>
       <c r="F1622" t="inlineStr">
@@ -59140,7 +59140,7 @@
       </c>
       <c r="G1622" t="inlineStr">
         <is>
-          <t>38,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1622" t="inlineStr">
@@ -59172,7 +59172,7 @@
       </c>
       <c r="E1623" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 16"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 2"</t>
         </is>
       </c>
       <c r="F1623" t="inlineStr">
@@ -59182,7 +59182,7 @@
       </c>
       <c r="G1623" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1623" t="inlineStr">
@@ -59214,7 +59214,7 @@
       </c>
       <c r="E1624" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 2"</t>
+          <t>SUMINISTRO DE NONMETALLIC FLAT GASKET, ARAMID FIBER REINFORCED NBR, ASME B16.21, THK 1/8", CLASS 150, FF, 2-1/2"</t>
         </is>
       </c>
       <c r="F1624" t="inlineStr">
@@ -59224,7 +59224,7 @@
       </c>
       <c r="G1624" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1624" t="inlineStr">
@@ -59266,7 +59266,7 @@
       </c>
       <c r="G1625" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>8,00</t>
         </is>
       </c>
       <c r="H1625" t="inlineStr">
@@ -59308,7 +59308,7 @@
       </c>
       <c r="G1626" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="H1626" t="inlineStr">
@@ -59350,7 +59350,7 @@
       </c>
       <c r="G1627" t="inlineStr">
         <is>
-          <t>44,00</t>
+          <t>20,00</t>
         </is>
       </c>
       <c r="H1627" t="inlineStr">
@@ -59392,7 +59392,7 @@
       </c>
       <c r="G1628" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1628" t="inlineStr">
@@ -59434,7 +59434,7 @@
       </c>
       <c r="G1629" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1629" t="inlineStr">
@@ -59466,7 +59466,7 @@
       </c>
       <c r="E1630" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 14"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 12"</t>
         </is>
       </c>
       <c r="F1630" t="inlineStr">
@@ -59476,7 +59476,7 @@
       </c>
       <c r="G1630" t="inlineStr">
         <is>
-          <t>34,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1630" t="inlineStr">
@@ -59508,7 +59508,7 @@
       </c>
       <c r="E1631" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 16"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 14"</t>
         </is>
       </c>
       <c r="F1631" t="inlineStr">
@@ -59518,7 +59518,7 @@
       </c>
       <c r="G1631" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="H1631" t="inlineStr">
@@ -59550,7 +59550,7 @@
       </c>
       <c r="E1632" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 24"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 16"</t>
         </is>
       </c>
       <c r="F1632" t="inlineStr">
@@ -59560,7 +59560,7 @@
       </c>
       <c r="G1632" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1632" t="inlineStr">
@@ -59592,7 +59592,7 @@
       </c>
       <c r="E1633" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 14"</t>
+          <t>SUMINISTRO DE SPIRAL WOUND GASKET ASME B16.20 _ 150 LB RAISED FACE _ 304 SS SPIRAL WOUND/GRAPHITE FILLER OUTER RING / FLEXITALLIC LS, 1/8" THK, 24"</t>
         </is>
       </c>
       <c r="F1633" t="inlineStr">
@@ -59602,7 +59602,7 @@
       </c>
       <c r="G1633" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>10,00</t>
         </is>
       </c>
       <c r="H1633" t="inlineStr">
@@ -59634,7 +59634,7 @@
       </c>
       <c r="E1634" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 16"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 14"</t>
         </is>
       </c>
       <c r="F1634" t="inlineStr">
@@ -59676,7 +59676,7 @@
       </c>
       <c r="E1635" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 3"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, GO, 16"</t>
         </is>
       </c>
       <c r="F1635" t="inlineStr">
@@ -59686,7 +59686,7 @@
       </c>
       <c r="G1635" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1635" t="inlineStr">
@@ -59718,7 +59718,7 @@
       </c>
       <c r="E1636" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 6"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 12"</t>
         </is>
       </c>
       <c r="F1636" t="inlineStr">
@@ -59728,7 +59728,7 @@
       </c>
       <c r="G1636" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1636" t="inlineStr">
@@ -59760,7 +59760,7 @@
       </c>
       <c r="E1637" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 8"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 3"</t>
         </is>
       </c>
       <c r="F1637" t="inlineStr">
@@ -59770,7 +59770,7 @@
       </c>
       <c r="G1637" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1637" t="inlineStr">
@@ -59802,7 +59802,7 @@
       </c>
       <c r="E1638" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 14"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 6"</t>
         </is>
       </c>
       <c r="F1638" t="inlineStr">
@@ -59812,7 +59812,7 @@
       </c>
       <c r="G1638" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1638" t="inlineStr">
@@ -59844,7 +59844,7 @@
       </c>
       <c r="E1639" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 16"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, API 600, API 598, A216 GR.WCB, CL 150, RF, B16.5, BB, SPW SS304/GRAPH, PKG GRAPH, TRIM #8, RENEWABLE SEATS, FLEXIBLE WEDGE, STEM OS&amp;Y/RSNRO, HO, 8"</t>
         </is>
       </c>
       <c r="F1639" t="inlineStr">
@@ -59854,7 +59854,7 @@
       </c>
       <c r="G1639" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1639" t="inlineStr">
@@ -59886,7 +59886,7 @@
       </c>
       <c r="E1640" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 2"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 14"</t>
         </is>
       </c>
       <c r="F1640" t="inlineStr">
@@ -59896,7 +59896,7 @@
       </c>
       <c r="G1640" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1640" t="inlineStr">
@@ -59928,7 +59928,7 @@
       </c>
       <c r="E1641" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 3"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 16"</t>
         </is>
       </c>
       <c r="F1641" t="inlineStr">
@@ -59938,7 +59938,7 @@
       </c>
       <c r="G1641" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1641" t="inlineStr">
@@ -59970,7 +59970,7 @@
       </c>
       <c r="E1642" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE HOSE GATE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREWED BONNET, PKG NON ASBESTOS, SOLID WEDGE, WEDGE B62, SEAT&amp;STEM BRONZE, NON RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 2"</t>
         </is>
       </c>
       <c r="F1642" t="inlineStr">
@@ -59980,7 +59980,7 @@
       </c>
       <c r="G1642" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1642" t="inlineStr">
@@ -60012,7 +60012,7 @@
       </c>
       <c r="E1643" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE ANGLE HOSE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREW-IN BONNET, RENEWABLE DISC, PKG NON ASBESTOS, DISC&amp;STEM BRONZE, RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 3"</t>
         </is>
       </c>
       <c r="F1643" t="inlineStr">
@@ -60022,7 +60022,7 @@
       </c>
       <c r="G1643" t="inlineStr">
         <is>
-          <t>48,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1643" t="inlineStr">
@@ -60054,7 +60054,7 @@
       </c>
       <c r="E1644" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 BExTE SEAMLESS ASTM A53 GR. B, 2-1/2", S-160</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 6"</t>
         </is>
       </c>
       <c r="F1644" t="inlineStr">
@@ -60064,7 +60064,7 @@
       </c>
       <c r="G1644" t="inlineStr">
         <is>
-          <t>60,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1644" t="inlineStr">
@@ -60096,7 +60096,7 @@
       </c>
       <c r="E1645" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
+          <t>SUMINISTRO DE GATE VALVE FL, MSS SP-128 TYPE II, A536 Gr 65-45-12, CL 125, FF, B16.1, BB, NON METALLIC FLAT GASKET EPDM, PKG EPDM, SOLID WEDGE, WEDGE DUCTILE IRON EPDM ENCAPSULATED, STEM BRONZE, OS&amp;Y/RSNRO, HO, UL LISTED/FM APPROVED, 8"</t>
         </is>
       </c>
       <c r="F1645" t="inlineStr">
@@ -60106,7 +60106,7 @@
       </c>
       <c r="G1645" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1645" t="inlineStr">
@@ -60138,7 +60138,7 @@
       </c>
       <c r="E1646" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
+          <t>SUMINISTRO DE HOSE GATE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREWED BONNET, PKG NON ASBESTOS, SOLID WEDGE, WEDGE B62, SEAT&amp;STEM BRONZE, NON RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
         </is>
       </c>
       <c r="F1646" t="inlineStr">
@@ -60148,7 +60148,7 @@
       </c>
       <c r="G1646" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1646" t="inlineStr">
@@ -60180,17 +60180,17 @@
       </c>
       <c r="E1647" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
+          <t>SUMINISTRO DE ANGLE HOSE VALVE THD, MSS SP-80, B62 UNS C83600, 300 PSI CWP, FNPT X NH W/CAP AND CHAIN, FNPT B1.20.1 AND NH NFPA 1963, SCREW-IN BONNET, RENEWABLE DISC, PKG NON ASBESTOS, DISC&amp;STEM BRONZE, RISING STEM, HO, UL LISTED/FM APPROVED, 2-1/2"</t>
         </is>
       </c>
       <c r="F1647" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1647" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1647" t="inlineStr">
@@ -60222,7 +60222,7 @@
       </c>
       <c r="E1648" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 6"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 BExTE SEAMLESS ASTM A53 GR. B, 2-1/2", S-160</t>
         </is>
       </c>
       <c r="F1648" t="inlineStr">
@@ -60232,7 +60232,7 @@
       </c>
       <c r="G1648" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>30,00</t>
         </is>
       </c>
       <c r="H1648" t="inlineStr">
@@ -60264,7 +60264,7 @@
       </c>
       <c r="E1649" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 14"X 8"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 1", S-80</t>
         </is>
       </c>
       <c r="F1649" t="inlineStr">
@@ -60274,7 +60274,7 @@
       </c>
       <c r="G1649" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1649" t="inlineStr">
@@ -60306,7 +60306,7 @@
       </c>
       <c r="E1650" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 3"</t>
+          <t>SUMINISTRO DE PIPE NIPPLE - LENGTH = 100 MM ASME B36.10 PE SEAMLESS ASTM A106 GR. B, 3/4", S-80</t>
         </is>
       </c>
       <c r="F1650" t="inlineStr">
@@ -60348,17 +60348,17 @@
       </c>
       <c r="E1651" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 14"X 12"</t>
+          <t>SUMINISTRO DE PIPE ASME B36.10 PE SEAMLESS ASTM A106 GR.  B, 1", S-80</t>
         </is>
       </c>
       <c r="F1651" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G1651" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1651" t="inlineStr">
@@ -60390,7 +60390,7 @@
       </c>
       <c r="E1652" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 14"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 20 X SCH 40, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 6"</t>
         </is>
       </c>
       <c r="F1652" t="inlineStr">
@@ -60400,7 +60400,7 @@
       </c>
       <c r="G1652" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1652" t="inlineStr">
@@ -60432,7 +60432,7 @@
       </c>
       <c r="E1653" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE REDUCER TEE, SCH20 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 4"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 30 X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 14"X 8"</t>
         </is>
       </c>
       <c r="F1653" t="inlineStr">
@@ -60442,7 +60442,7 @@
       </c>
       <c r="G1653" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1653" t="inlineStr">
@@ -60474,7 +60474,7 @@
       </c>
       <c r="E1654" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 24" X 3/4"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH 40 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 6"X 3"</t>
         </is>
       </c>
       <c r="F1654" t="inlineStr">
@@ -60484,7 +60484,7 @@
       </c>
       <c r="G1654" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1654" t="inlineStr">
@@ -60516,7 +60516,7 @@
       </c>
       <c r="E1655" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 8" X 3/4"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH STD X SCH 20, BW, ASTM A-234 GR WPB, ASME B16.9 14"X 12"</t>
         </is>
       </c>
       <c r="F1655" t="inlineStr">
@@ -60558,7 +60558,7 @@
       </c>
       <c r="E1656" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"X 14"</t>
         </is>
       </c>
       <c r="F1656" t="inlineStr">
@@ -60600,7 +60600,7 @@
       </c>
       <c r="E1657" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
+          <t>SUMINISTRO DE REDUCER TEE, SCH20 X SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 8"X 4"</t>
         </is>
       </c>
       <c r="F1657" t="inlineStr">
@@ -60610,7 +60610,7 @@
       </c>
       <c r="G1657" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1657" t="inlineStr">
@@ -60642,7 +60642,7 @@
       </c>
       <c r="E1658" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 2-1/2"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 24" X 3/4"</t>
         </is>
       </c>
       <c r="F1658" t="inlineStr">
@@ -60652,7 +60652,7 @@
       </c>
       <c r="G1658" t="inlineStr">
         <is>
-          <t>14,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1658" t="inlineStr">
@@ -60684,7 +60684,7 @@
       </c>
       <c r="E1659" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 24"</t>
+          <t>SUMINISTRO DE SOCKOLET MSS SP-97 BW X SW 3000# FORGED ASTM A105, 8" X 3/4"</t>
         </is>
       </c>
       <c r="F1659" t="inlineStr">
@@ -60694,7 +60694,7 @@
       </c>
       <c r="G1659" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1659" t="inlineStr">
@@ -60726,7 +60726,7 @@
       </c>
       <c r="E1660" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
+          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 10"</t>
         </is>
       </c>
       <c r="F1660" t="inlineStr">
@@ -60736,7 +60736,7 @@
       </c>
       <c r="G1660" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1660" t="inlineStr">
@@ -60768,7 +60768,7 @@
       </c>
       <c r="E1661" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"</t>
+          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
         </is>
       </c>
       <c r="F1661" t="inlineStr">
@@ -60778,7 +60778,7 @@
       </c>
       <c r="G1661" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1661" t="inlineStr">
@@ -60810,7 +60810,7 @@
       </c>
       <c r="E1662" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 10"</t>
+          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 2-1/2"</t>
         </is>
       </c>
       <c r="F1662" t="inlineStr">
@@ -60820,7 +60820,7 @@
       </c>
       <c r="G1662" t="inlineStr">
         <is>
-          <t>28,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="H1662" t="inlineStr">
@@ -60852,7 +60852,7 @@
       </c>
       <c r="E1663" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 14"</t>
+          <t>SUMINISTRO DE TEE, SCH 30, BW, ASTM A-234 GR WPB, ASME B16.9 24"</t>
         </is>
       </c>
       <c r="F1663" t="inlineStr">
@@ -60862,7 +60862,7 @@
       </c>
       <c r="G1663" t="inlineStr">
         <is>
-          <t>48,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1663" t="inlineStr">
@@ -60894,7 +60894,7 @@
       </c>
       <c r="E1664" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 24"</t>
+          <t>SUMINISTRO DE TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 14"</t>
         </is>
       </c>
       <c r="F1664" t="inlineStr">
@@ -60904,7 +60904,7 @@
       </c>
       <c r="G1664" t="inlineStr">
         <is>
-          <t>28,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1664" t="inlineStr">
@@ -60936,7 +60936,7 @@
       </c>
       <c r="E1665" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 40, RF, ASTM A-105, ASME B16.5 16"</t>
+          <t>SUMINISTRO DE TEE, SCH STD, BW, ASTM A-234 GR WPB, ASME B16.9 16"</t>
         </is>
       </c>
       <c r="F1665" t="inlineStr">
@@ -60946,7 +60946,7 @@
       </c>
       <c r="G1665" t="inlineStr">
         <is>
-          <t>12,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1665" t="inlineStr">
@@ -60978,7 +60978,7 @@
       </c>
       <c r="E1666" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 12", S-20</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 10"</t>
         </is>
       </c>
       <c r="F1666" t="inlineStr">
@@ -60988,7 +60988,7 @@
       </c>
       <c r="G1666" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1666" t="inlineStr">
@@ -61020,7 +61020,7 @@
       </c>
       <c r="E1667" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 14", S-STD</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 12"</t>
         </is>
       </c>
       <c r="F1667" t="inlineStr">
@@ -61030,7 +61030,7 @@
       </c>
       <c r="G1667" t="inlineStr">
         <is>
-          <t>50,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1667" t="inlineStr">
@@ -61062,7 +61062,7 @@
       </c>
       <c r="E1668" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 16", S-STD</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 14"</t>
         </is>
       </c>
       <c r="F1668" t="inlineStr">
@@ -61072,7 +61072,7 @@
       </c>
       <c r="G1668" t="inlineStr">
         <is>
-          <t>32,00</t>
+          <t>24,00</t>
         </is>
       </c>
       <c r="H1668" t="inlineStr">
@@ -61104,7 +61104,7 @@
       </c>
       <c r="E1669" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 3", S-30</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 30, RF, ASTM A-105, ASME B16.5 24"</t>
         </is>
       </c>
       <c r="F1669" t="inlineStr">
@@ -61114,7 +61114,7 @@
       </c>
       <c r="G1669" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1669" t="inlineStr">
@@ -61146,7 +61146,7 @@
       </c>
       <c r="E1670" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 4", S-30</t>
+          <t>SUMINISTRO DE FLANGE WN, 150#, SCH 40, RF, ASTM A-105, ASME B16.5 16"</t>
         </is>
       </c>
       <c r="F1670" t="inlineStr">
@@ -61156,7 +61156,7 @@
       </c>
       <c r="G1670" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="H1670" t="inlineStr">
@@ -61188,7 +61188,7 @@
       </c>
       <c r="E1671" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 8", S-20</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 12", S-20</t>
         </is>
       </c>
       <c r="F1671" t="inlineStr">
@@ -61198,7 +61198,7 @@
       </c>
       <c r="G1671" t="inlineStr">
         <is>
-          <t>30,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="H1671" t="inlineStr">
@@ -61230,7 +61230,7 @@
       </c>
       <c r="E1672" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 14" X 2-1/2", S-STD X S-30</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 14", S-STD</t>
         </is>
       </c>
       <c r="F1672" t="inlineStr">
@@ -61240,7 +61240,7 @@
       </c>
       <c r="G1672" t="inlineStr">
         <is>
-          <t>34,00</t>
+          <t>25,00</t>
         </is>
       </c>
       <c r="H1672" t="inlineStr">
@@ -61272,7 +61272,7 @@
       </c>
       <c r="E1673" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 10", S-30 X S-30</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 16", S-STD</t>
         </is>
       </c>
       <c r="F1673" t="inlineStr">
@@ -61282,7 +61282,7 @@
       </c>
       <c r="G1673" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>14,00</t>
         </is>
       </c>
       <c r="H1673" t="inlineStr">
@@ -61314,7 +61314,7 @@
       </c>
       <c r="E1674" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 2", S-30 X S-40</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 2-1/2", S-30</t>
         </is>
       </c>
       <c r="F1674" t="inlineStr">
@@ -61324,7 +61324,7 @@
       </c>
       <c r="G1674" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1674" t="inlineStr">
@@ -61356,7 +61356,7 @@
       </c>
       <c r="E1675" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 3", S-30 X S-40</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 3", S-30</t>
         </is>
       </c>
       <c r="F1675" t="inlineStr">
@@ -61366,7 +61366,7 @@
       </c>
       <c r="G1675" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1675" t="inlineStr">
@@ -61398,7 +61398,7 @@
       </c>
       <c r="E1676" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 4", S-30 X S-40</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 4", S-30</t>
         </is>
       </c>
       <c r="F1676" t="inlineStr">
@@ -61408,7 +61408,7 @@
       </c>
       <c r="G1676" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="H1676" t="inlineStr">
@@ -61440,7 +61440,7 @@
       </c>
       <c r="E1677" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 6" X 2-1/2", S-40 X S-30</t>
+          <t>SUMINISTRO DE WELDNECK FLANGE ASME B16.5 FLG X BW 150 LB FLAT FACE FORGED ASTM A105, 8", S-20</t>
         </is>
       </c>
       <c r="F1677" t="inlineStr">
@@ -61450,7 +61450,7 @@
       </c>
       <c r="G1677" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="H1677" t="inlineStr">
@@ -61482,7 +61482,7 @@
       </c>
       <c r="E1678" t="inlineStr">
         <is>
-          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 8" X 2", S-20 X S-40</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 14" X 2-1/2", S-STD X S-30</t>
         </is>
       </c>
       <c r="F1678" t="inlineStr">
@@ -61492,7 +61492,7 @@
       </c>
       <c r="G1678" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="H1678" t="inlineStr">
@@ -61524,17 +61524,17 @@
       </c>
       <c r="E1679" t="inlineStr">
         <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES BRIDADAS ANSI 150 DE DIAMETRO 2-1/2"</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 14" X 6", S-STD X S-40</t>
         </is>
       </c>
       <c r="F1679" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1679" t="inlineStr">
         <is>
-          <t>54,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="H1679" t="inlineStr">
@@ -61566,17 +61566,17 @@
       </c>
       <c r="E1680" t="inlineStr">
         <is>
-          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 10", S-30 X S-30</t>
         </is>
       </c>
       <c r="F1680" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1680" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="H1680" t="inlineStr">
@@ -61608,17 +61608,17 @@
       </c>
       <c r="E1681" t="inlineStr">
         <is>
-          <t>MONTAJE AÉREO DE TUBERÍA DE Ø 2-1/2" (SIN PREFABRICAR)</t>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 2", S-30 X S-40</t>
         </is>
       </c>
       <c r="F1681" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="G1681" t="inlineStr">
         <is>
-          <t>136,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="H1681" t="inlineStr">
@@ -61650,20 +61650,314 @@
       </c>
       <c r="E1682" t="inlineStr">
         <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 3", S-30 X S-40</t>
+        </is>
+      </c>
+      <c r="F1682" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1682" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1682" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1683">
+      <c r="A1683" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1683" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1683" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1683" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1683" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 24" X 4", S-30 X S-40</t>
+        </is>
+      </c>
+      <c r="F1683" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1683" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H1683" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1684">
+      <c r="A1684" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1684" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1684" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1684" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1684" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 6" X 2-1/2", S-40 X S-30</t>
+        </is>
+      </c>
+      <c r="F1684" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1684" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="H1684" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1685">
+      <c r="A1685" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1685" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1685" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1685" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1685" t="inlineStr">
+        <is>
+          <t>SUMINISTRO DE WELDOLET MSS SP-97 BW X BW FORGED ASTM A105, 8" X 2", S-20 X S-40</t>
+        </is>
+      </c>
+      <c r="F1685" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="G1685" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="H1685" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1686">
+      <c r="A1686" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1686" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1686" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1686" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1686" t="inlineStr">
+        <is>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES BRIDADAS ANSI 150 DE DIAMETRO 2-1/2"</t>
+        </is>
+      </c>
+      <c r="F1686" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1686" t="inlineStr">
+        <is>
+          <t>27,00</t>
+        </is>
+      </c>
+      <c r="H1686" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1687">
+      <c r="A1687" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1687" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1687" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1687" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1687" t="inlineStr">
+        <is>
+          <t>PRUEBAS HIDROSTATICAS DE VÁLVULAS MANUALES SW 800# DE DIAMETRO MENORES 2"</t>
+        </is>
+      </c>
+      <c r="F1687" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1687" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="H1687" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1688">
+      <c r="A1688" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1688" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1688" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1688" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1688" t="inlineStr">
+        <is>
+          <t>MONTAJE AÉREO DE TUBERÍA DE Ø 2-1/2" (SIN PREFABRICAR)</t>
+        </is>
+      </c>
+      <c r="F1688" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1688" t="inlineStr">
+        <is>
+          <t>75,00</t>
+        </is>
+      </c>
+      <c r="H1688" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1689">
+      <c r="A1689" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B1689" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C1689" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1689" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E1689" t="inlineStr">
+        <is>
           <t>MONTAJE DE VÁLVULAS Y CHEQUES DIAMETRO DE 2-1/2"</t>
         </is>
       </c>
-      <c r="F1682" t="inlineStr">
+      <c r="F1689" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G1682" t="inlineStr">
-        <is>
-          <t>54,00</t>
-        </is>
-      </c>
-      <c r="H1682" t="inlineStr">
+      <c r="G1689" t="inlineStr">
+        <is>
+          <t>27,00</t>
+        </is>
+      </c>
+      <c r="H1689" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>

</xml_diff>